<commit_message>
Upload aller aktuellen Dokumente
</commit_message>
<xml_diff>
--- a/website/src/documents/allgemein/Apollon_Projektplan.xlsx
+++ b/website/src/documents/allgemein/Apollon_Projektplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dhbwstg.sharepoint.com/sites/o365grpSWE-Projekt/Freigegebene Dokumente/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="596" documentId="8_{45909616-94BE-491C-BFA5-6DC92E6FFB12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B8B15BF1-0275-4212-A299-42E192A1A01C}"/>
+  <xr:revisionPtr revIDLastSave="766" documentId="8_{45909616-94BE-491C-BFA5-6DC92E6FFB12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B538BEDB-447C-4491-925E-EE717C4FD712}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{5DFA726E-B0C4-4500-AF96-5BC0FDCBA0B9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="7" xr2:uid="{5DFA726E-B0C4-4500-AF96-5BC0FDCBA0B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Zielsetzung" sheetId="5" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Initialisierungsphase" sheetId="2" r:id="rId5"/>
     <sheet name="Recherchephase" sheetId="4" r:id="rId6"/>
     <sheet name="Einarbeitungsphase" sheetId="7" r:id="rId7"/>
+    <sheet name="Anforderungsanalyse" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="148">
   <si>
     <r>
       <t xml:space="preserve">Zielsetzung
@@ -498,6 +499,66 @@
   </si>
   <si>
     <t>Erste Version des Glossars</t>
+  </si>
+  <si>
+    <t>Entwurf der Spielelogik</t>
+  </si>
+  <si>
+    <t>10h</t>
+  </si>
+  <si>
+    <t>Designstudie</t>
+  </si>
+  <si>
+    <t>Dokumentations-Richtlinien</t>
+  </si>
+  <si>
+    <t>Dokumentationskonzept</t>
+  </si>
+  <si>
+    <t>Verantwortlicher für Qualtitätsmanagement | Daniel Kröker</t>
+  </si>
+  <si>
+    <t>Erstellen der Dungeon-Konfiguration</t>
+  </si>
+  <si>
+    <t>Erstellen der Spieleansicht</t>
+  </si>
+  <si>
+    <t>Erstellen eines Chatsystems</t>
+  </si>
+  <si>
+    <t>Erstellen einer Übersichtsseite</t>
+  </si>
+  <si>
+    <t>Erstellen einer Login-Systems</t>
+  </si>
+  <si>
+    <t>Verantwortung übernommen von Leon Jerke</t>
+  </si>
+  <si>
+    <t>Verantwortlicher für Modellierung | Etienne Zink</t>
+  </si>
+  <si>
+    <t>20h</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>Übertragen des Lastenhefts</t>
+  </si>
+  <si>
+    <t>Zeichnen der UML-Diagramme</t>
+  </si>
+  <si>
+    <t>Absprechen mit dem Kunden</t>
+  </si>
+  <si>
+    <t>Überarbeitung und Erweiterung des Glossars</t>
+  </si>
+  <si>
+    <t>3h</t>
   </si>
 </sst>
 </file>
@@ -695,7 +756,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="112">
+  <borders count="120">
     <border>
       <left/>
       <right/>
@@ -1979,21 +2040,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="0"/>
       </left>
@@ -2132,11 +2178,118 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="221">
+  <cellXfs count="246">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2585,88 +2738,136 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="96" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="97" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="98" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="101" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="103" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="104" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="105" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="106" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="101" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="96" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="97" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="98" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="101" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="104" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="103" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="105" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="106" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="111" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="114" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="116" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2705,12 +2906,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2778,6 +2979,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="117" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="118" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="119" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4186,6 +4414,116 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>821094</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>420614</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>821094</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>238760</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Gerader Verbinder 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BED0460-6707-4E63-953A-3CDCFF735B89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10901029" y="4595049"/>
+          <a:ext cx="0" cy="248841"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="3FB3DA"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>832689</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1514</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>832689</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1876</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Gerader Verbinder 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB733015-4082-4DD7-BD8B-139FFBD209B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10912624" y="5244405"/>
+          <a:ext cx="0" cy="248841"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="3FB3DA"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4547,11 +4885,11 @@
     </row>
     <row r="3" spans="1:15" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
-      <c r="B3" s="184" t="s">
+      <c r="B3" s="200" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="185"/>
-      <c r="D3" s="186"/>
+      <c r="C3" s="201"/>
+      <c r="D3" s="202"/>
       <c r="E3" s="101"/>
       <c r="F3" s="101"/>
       <c r="G3" s="101"/>
@@ -4566,11 +4904,11 @@
     </row>
     <row r="4" spans="1:15" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="112"/>
-      <c r="B4" s="187" t="s">
+      <c r="B4" s="203" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="188"/>
-      <c r="D4" s="189"/>
+      <c r="C4" s="204"/>
+      <c r="D4" s="205"/>
       <c r="E4" s="103"/>
       <c r="F4" s="103"/>
       <c r="G4" s="103"/>
@@ -4585,9 +4923,9 @@
     </row>
     <row r="5" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="112"/>
-      <c r="B5" s="190"/>
-      <c r="C5" s="191"/>
-      <c r="D5" s="192"/>
+      <c r="B5" s="206"/>
+      <c r="C5" s="207"/>
+      <c r="D5" s="208"/>
       <c r="E5" s="103"/>
       <c r="F5" s="103"/>
       <c r="G5" s="103"/>
@@ -4602,9 +4940,9 @@
     </row>
     <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="112"/>
-      <c r="B6" s="190"/>
-      <c r="C6" s="191"/>
-      <c r="D6" s="192"/>
+      <c r="B6" s="206"/>
+      <c r="C6" s="207"/>
+      <c r="D6" s="208"/>
       <c r="E6" s="103"/>
       <c r="F6" s="103"/>
       <c r="G6" s="103"/>
@@ -4619,9 +4957,9 @@
     </row>
     <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="112"/>
-      <c r="B7" s="190"/>
-      <c r="C7" s="191"/>
-      <c r="D7" s="192"/>
+      <c r="B7" s="206"/>
+      <c r="C7" s="207"/>
+      <c r="D7" s="208"/>
       <c r="E7" s="103"/>
       <c r="F7" s="103"/>
       <c r="G7" s="103"/>
@@ -4636,9 +4974,9 @@
     </row>
     <row r="8" spans="1:15" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="112"/>
-      <c r="B8" s="190"/>
-      <c r="C8" s="191"/>
-      <c r="D8" s="192"/>
+      <c r="B8" s="206"/>
+      <c r="C8" s="207"/>
+      <c r="D8" s="208"/>
       <c r="E8" s="103"/>
       <c r="F8" s="103"/>
       <c r="G8" s="103"/>
@@ -4653,9 +4991,9 @@
     </row>
     <row r="9" spans="1:15" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="112"/>
-      <c r="B9" s="193"/>
-      <c r="C9" s="194"/>
-      <c r="D9" s="195"/>
+      <c r="B9" s="209"/>
+      <c r="C9" s="210"/>
+      <c r="D9" s="211"/>
       <c r="E9" s="103"/>
       <c r="F9" s="103"/>
       <c r="G9" s="103"/>
@@ -5612,7 +5950,7 @@
   <dimension ref="A2:AB44"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5652,32 +5990,32 @@
       <c r="G3" s="130"/>
     </row>
     <row r="4" spans="1:13" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="158"/>
-      <c r="E4" s="157"/>
-      <c r="F4" s="196" t="s">
+      <c r="D4" s="157"/>
+      <c r="E4" s="156"/>
+      <c r="F4" s="212" t="s">
         <v>99</v>
       </c>
-      <c r="G4" s="197"/>
-      <c r="H4" s="180"/>
-      <c r="I4" s="158"/>
-      <c r="J4" s="158"/>
+      <c r="G4" s="213"/>
+      <c r="H4" s="178"/>
+      <c r="I4" s="157"/>
+      <c r="J4" s="157"/>
     </row>
     <row r="5" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="160"/>
-      <c r="C5" s="181"/>
-      <c r="D5" s="159"/>
+      <c r="B5" s="159"/>
+      <c r="C5" s="179"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="132"/>
       <c r="F5" s="132"/>
       <c r="G5" s="132"/>
       <c r="H5" s="132"/>
       <c r="I5" s="132"/>
-      <c r="J5" s="179"/>
-      <c r="K5" s="178"/>
-      <c r="L5" s="158"/>
+      <c r="J5" s="177"/>
+      <c r="K5" s="176"/>
+      <c r="L5" s="157"/>
     </row>
     <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="114"/>
-      <c r="B6" s="161"/>
+      <c r="B6" s="160"/>
       <c r="C6" s="131"/>
       <c r="D6" s="131"/>
       <c r="E6" s="131"/>
@@ -5687,20 +6025,20 @@
       <c r="I6" s="131"/>
       <c r="J6" s="148"/>
       <c r="K6" s="131"/>
-      <c r="L6" s="177"/>
+      <c r="L6" s="175"/>
       <c r="M6" s="22"/>
     </row>
     <row r="7" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="114"/>
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="161" t="s">
         <v>100</v>
       </c>
       <c r="C7" s="146"/>
-      <c r="D7" s="198" t="s">
+      <c r="D7" s="214" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="199"/>
-      <c r="F7" s="200"/>
+      <c r="E7" s="215"/>
+      <c r="F7" s="216"/>
       <c r="G7" s="146"/>
       <c r="H7" s="145" t="s">
         <v>102</v>
@@ -5710,14 +6048,14 @@
         <v>111</v>
       </c>
       <c r="K7" s="146"/>
-      <c r="L7" s="172" t="s">
+      <c r="L7" s="170" t="s">
         <v>103</v>
       </c>
       <c r="M7" s="22"/>
     </row>
     <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="114"/>
-      <c r="B8" s="163"/>
+      <c r="B8" s="162"/>
       <c r="C8" s="133"/>
       <c r="D8" s="135"/>
       <c r="E8" s="135"/>
@@ -5726,12 +6064,12 @@
       <c r="H8" s="134"/>
       <c r="I8" s="134"/>
       <c r="J8" s="134"/>
-      <c r="L8" s="167"/>
+      <c r="L8" s="166"/>
       <c r="M8" s="22"/>
     </row>
     <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="114"/>
-      <c r="B9" s="164"/>
+      <c r="B9" s="163"/>
       <c r="C9" s="137"/>
       <c r="D9" s="142"/>
       <c r="E9" s="142"/>
@@ -5740,12 +6078,12 @@
       <c r="H9" s="135"/>
       <c r="I9" s="134"/>
       <c r="J9" s="135"/>
-      <c r="L9" s="173"/>
+      <c r="L9" s="171"/>
       <c r="M9" s="22"/>
     </row>
     <row r="10" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="167"/>
-      <c r="B10" s="165" t="s">
+      <c r="A10" s="166"/>
+      <c r="B10" s="164" t="s">
         <v>105</v>
       </c>
       <c r="C10" s="139"/>
@@ -5763,14 +6101,14 @@
         <v>114</v>
       </c>
       <c r="K10" s="141"/>
-      <c r="L10" s="174" t="s">
+      <c r="L10" s="172" t="s">
         <v>115</v>
       </c>
       <c r="M10" s="22"/>
     </row>
     <row r="11" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="167"/>
-      <c r="B11" s="166"/>
+      <c r="A11" s="166"/>
+      <c r="B11" s="165"/>
       <c r="C11" s="134"/>
       <c r="D11" s="140"/>
       <c r="E11" s="140"/>
@@ -5779,12 +6117,12 @@
       <c r="H11" s="140"/>
       <c r="I11" s="134"/>
       <c r="J11" s="133"/>
-      <c r="L11" s="175"/>
+      <c r="L11" s="173"/>
       <c r="M11" s="22"/>
     </row>
     <row r="12" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="167"/>
-      <c r="B12" s="165" t="s">
+      <c r="A12" s="166"/>
+      <c r="B12" s="164" t="s">
         <v>67</v>
       </c>
       <c r="C12" s="137"/>
@@ -5806,13 +6144,13 @@
         <v>113</v>
       </c>
       <c r="K12" s="114"/>
-      <c r="L12" s="174" t="s">
+      <c r="L12" s="172" t="s">
         <v>116</v>
       </c>
       <c r="M12" s="22"/>
     </row>
     <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="167"/>
+      <c r="A13" s="166"/>
       <c r="B13" s="136"/>
       <c r="C13" s="134"/>
       <c r="D13" s="133"/>
@@ -5822,12 +6160,12 @@
       <c r="H13" s="140"/>
       <c r="I13" s="134"/>
       <c r="J13" s="134"/>
-      <c r="L13" s="175"/>
+      <c r="L13" s="173"/>
       <c r="M13" s="22"/>
     </row>
     <row r="14" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="167"/>
-      <c r="B14" s="165" t="s">
+      <c r="A14" s="166"/>
+      <c r="B14" s="164" t="s">
         <v>104</v>
       </c>
       <c r="C14" s="134"/>
@@ -5841,13 +6179,13 @@
       <c r="I14" s="136"/>
       <c r="J14" s="134"/>
       <c r="K14" s="114"/>
-      <c r="L14" s="174" t="s">
+      <c r="L14" s="172" t="s">
         <v>117</v>
       </c>
       <c r="M14" s="22"/>
     </row>
     <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="167"/>
+      <c r="A15" s="166"/>
       <c r="B15" s="136"/>
       <c r="C15" s="134"/>
       <c r="D15" s="134"/>
@@ -5857,29 +6195,25 @@
       <c r="H15" s="140"/>
       <c r="I15" s="134"/>
       <c r="J15" s="134"/>
-      <c r="L15" s="176"/>
+      <c r="L15" s="174"/>
       <c r="M15" s="22"/>
     </row>
-    <row r="16" spans="1:13" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="167"/>
-      <c r="B16" s="168" t="s">
+    <row r="16" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="166"/>
+      <c r="B16" s="194" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="169"/>
-      <c r="D16" s="169"/>
-      <c r="E16" s="169"/>
-      <c r="F16" s="169"/>
-      <c r="G16" s="170"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="171"/>
-      <c r="J16" s="169"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="157"/>
+      <c r="G16" s="114"/>
+      <c r="H16" s="196" t="s">
+        <v>131</v>
+      </c>
+      <c r="L16" s="171"/>
       <c r="M16" s="22"/>
     </row>
-    <row r="17" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
+    <row r="17" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="189"/>
+      <c r="B17" s="190"/>
+      <c r="C17" s="191"/>
       <c r="D17" s="47"/>
       <c r="E17" s="47"/>
       <c r="F17" s="47"/>
@@ -5888,13 +6222,35 @@
       <c r="I17" s="47"/>
       <c r="J17" s="47"/>
       <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-    </row>
-    <row r="30" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L17" s="171"/>
+    </row>
+    <row r="18" spans="1:22" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="189"/>
+      <c r="B18" s="192"/>
+      <c r="C18" s="193"/>
+      <c r="D18" s="167"/>
+      <c r="E18" s="167"/>
+      <c r="F18" s="167"/>
+      <c r="G18" s="168"/>
+      <c r="H18" s="195" t="s">
+        <v>130</v>
+      </c>
+      <c r="I18" s="169"/>
+      <c r="J18" s="167"/>
+      <c r="K18" s="157"/>
+      <c r="L18" s="156"/>
+    </row>
+    <row r="20" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="130"/>
+    </row>
+    <row r="21" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="47"/>
+    </row>
+    <row r="30" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U30" s="130"/>
       <c r="V30" s="130"/>
     </row>
-    <row r="31" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="15:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P33" s="114"/>
       <c r="AB33" s="22"/>
@@ -7860,7 +8216,7 @@
     </row>
     <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71"/>
-      <c r="B4" s="205" t="s">
+      <c r="B4" s="221" t="s">
         <v>58</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -7869,48 +8225,48 @@
       <c r="D4" s="123" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="208" t="s">
+      <c r="E4" s="224" t="s">
         <v>61</v>
       </c>
       <c r="F4" s="123"/>
-      <c r="G4" s="209" t="s">
+      <c r="G4" s="225" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="210" t="s">
+      <c r="H4" s="226" t="s">
         <v>62</v>
       </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
-      <c r="B5" s="206"/>
+      <c r="B5" s="222"/>
       <c r="C5" s="7" t="s">
         <v>63</v>
       </c>
       <c r="D5" s="123" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="208"/>
+      <c r="E5" s="224"/>
       <c r="F5" s="123"/>
-      <c r="G5" s="209"/>
-      <c r="H5" s="210"/>
+      <c r="G5" s="225"/>
+      <c r="H5" s="226"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="71"/>
-      <c r="B6" s="207"/>
+      <c r="B6" s="223"/>
       <c r="C6" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D6" s="123" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="208"/>
+      <c r="E6" s="224"/>
       <c r="F6" s="123" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="209"/>
-      <c r="H6" s="210"/>
+      <c r="G6" s="225"/>
+      <c r="H6" s="226"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8003,13 +8359,13 @@
     </row>
     <row r="11" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="71"/>
-      <c r="B11" s="211" t="s">
+      <c r="B11" s="227" t="s">
         <v>84</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="215" t="s">
+      <c r="D11" s="231" t="s">
         <v>73</v>
       </c>
       <c r="E11" s="127" t="s">
@@ -8026,11 +8382,11 @@
     </row>
     <row r="12" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="71"/>
-      <c r="B12" s="213"/>
+      <c r="B12" s="229"/>
       <c r="C12" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="216"/>
+      <c r="D12" s="232"/>
       <c r="E12" s="127" t="s">
         <v>69</v>
       </c>
@@ -8045,11 +8401,11 @@
     </row>
     <row r="13" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="71"/>
-      <c r="B13" s="214"/>
+      <c r="B13" s="230"/>
       <c r="C13" s="127" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="217"/>
+      <c r="D13" s="233"/>
       <c r="E13" s="127" t="s">
         <v>89</v>
       </c>
@@ -8079,14 +8435,14 @@
       <c r="F14" s="149" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="218" t="s">
+      <c r="G14" s="234" t="s">
         <v>57</v>
       </c>
-      <c r="H14" s="219"/>
+      <c r="H14" s="235"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="211" t="s">
+      <c r="B15" s="227" t="s">
         <v>77</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -8101,13 +8457,13 @@
       <c r="F15" s="123" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="203" t="s">
+      <c r="G15" s="219" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="204"/>
+      <c r="H15" s="220"/>
     </row>
     <row r="16" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="212"/>
+      <c r="B16" s="228"/>
       <c r="C16" s="7" t="s">
         <v>82</v>
       </c>
@@ -8118,10 +8474,10 @@
         <v>83</v>
       </c>
       <c r="F16" s="123"/>
-      <c r="G16" s="203" t="s">
+      <c r="G16" s="219" t="s">
         <v>62</v>
       </c>
-      <c r="H16" s="204"/>
+      <c r="H16" s="220"/>
     </row>
     <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="153" t="s">
@@ -8135,10 +8491,10 @@
         <v>71</v>
       </c>
       <c r="F17" s="155"/>
-      <c r="G17" s="201" t="s">
+      <c r="G17" s="217" t="s">
         <v>75</v>
       </c>
-      <c r="H17" s="202"/>
+      <c r="H17" s="218"/>
     </row>
     <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
@@ -8237,7 +8593,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8302,7 +8658,7 @@
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="71"/>
-      <c r="B4" s="220" t="s">
+      <c r="B4" s="236" t="s">
         <v>90</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -8313,17 +8669,17 @@
       </c>
       <c r="E4" s="123"/>
       <c r="F4" s="123"/>
-      <c r="G4" s="209" t="s">
+      <c r="G4" s="225" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="182" t="s">
+      <c r="H4" s="180" t="s">
         <v>62</v>
       </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
-      <c r="B5" s="220"/>
+      <c r="B5" s="236"/>
       <c r="C5" s="7" t="s">
         <v>122</v>
       </c>
@@ -8332,15 +8688,15 @@
       </c>
       <c r="E5" s="123"/>
       <c r="F5" s="123"/>
-      <c r="G5" s="209"/>
-      <c r="H5" s="182" t="s">
+      <c r="G5" s="225"/>
+      <c r="H5" s="180" t="s">
         <v>62</v>
       </c>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="71"/>
-      <c r="B6" s="220"/>
+      <c r="B6" s="236"/>
       <c r="C6" s="7" t="s">
         <v>123</v>
       </c>
@@ -8349,15 +8705,15 @@
       </c>
       <c r="E6" s="123"/>
       <c r="F6" s="123"/>
-      <c r="G6" s="209"/>
-      <c r="H6" s="182" t="s">
+      <c r="G6" s="225"/>
+      <c r="H6" s="180" t="s">
         <v>62</v>
       </c>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="71"/>
-      <c r="B7" s="220"/>
+      <c r="B7" s="236"/>
       <c r="C7" s="7" t="s">
         <v>91</v>
       </c>
@@ -8366,8 +8722,8 @@
       </c>
       <c r="E7" s="123"/>
       <c r="F7" s="123"/>
-      <c r="G7" s="209"/>
-      <c r="H7" s="182" t="s">
+      <c r="G7" s="225"/>
+      <c r="H7" s="180" t="s">
         <v>62</v>
       </c>
       <c r="I7" s="3"/>
@@ -8389,10 +8745,10 @@
       <c r="F8" s="149" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="218" t="s">
+      <c r="G8" s="234" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="219"/>
+      <c r="H8" s="235"/>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8408,10 +8764,10 @@
         <v>71</v>
       </c>
       <c r="F9" s="155"/>
-      <c r="G9" s="201" t="s">
+      <c r="G9" s="217" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="202"/>
+      <c r="H9" s="218"/>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -8527,10 +8883,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE2F811-FC50-4C49-9F73-322F02BE8356}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8540,7 +8896,446 @@
     <col min="3" max="3" width="42.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="34.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+    </row>
+    <row r="2" spans="1:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="71"/>
+      <c r="B2" s="75" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="92"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="71"/>
+      <c r="B3" s="95" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="77" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="76" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="76" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="78" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="71"/>
+      <c r="B4" s="227" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="231" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="231" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="231" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" s="239" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="184" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="71"/>
+      <c r="B5" s="229"/>
+      <c r="C5" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="232"/>
+      <c r="E5" s="232"/>
+      <c r="F5" s="232"/>
+      <c r="G5" s="240"/>
+      <c r="H5" s="184" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="71"/>
+      <c r="B6" s="229"/>
+      <c r="C6" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="232"/>
+      <c r="E6" s="232"/>
+      <c r="F6" s="232"/>
+      <c r="G6" s="240"/>
+      <c r="H6" s="184" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="71"/>
+      <c r="B7" s="229"/>
+      <c r="C7" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="232"/>
+      <c r="E7" s="232"/>
+      <c r="F7" s="232"/>
+      <c r="G7" s="240"/>
+      <c r="H7" s="184" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="71"/>
+      <c r="B8" s="228"/>
+      <c r="C8" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="238"/>
+      <c r="E8" s="238"/>
+      <c r="F8" s="238"/>
+      <c r="G8" s="241"/>
+      <c r="H8" s="129" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="71"/>
+      <c r="B9" s="181" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="127" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="127" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" s="127"/>
+      <c r="G9" s="183" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="129" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="71"/>
+      <c r="B10" s="186" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="182" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="182" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="182"/>
+      <c r="G10" s="183"/>
+      <c r="H10" s="184" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="71"/>
+      <c r="B11" s="181" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="127" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="127" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="127"/>
+      <c r="G11" s="128" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="129" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="71"/>
+      <c r="B12" s="186" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="182" t="s">
+        <v>133</v>
+      </c>
+      <c r="E12" s="182" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="182"/>
+      <c r="G12" s="183" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="184" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="71"/>
+      <c r="B13" s="186" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="185" t="s">
+        <v>140</v>
+      </c>
+      <c r="E13" s="185" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13" s="185"/>
+      <c r="G13" s="183" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="184" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="71"/>
+      <c r="B14" s="150" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="197" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="199" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="199" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="199" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="237" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="235"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="71"/>
+      <c r="B15" s="153" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="154"/>
+      <c r="D15" s="198" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="198" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="198"/>
+      <c r="G15" s="217" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="218"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="87"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="89"/>
+      <c r="H16" s="74"/>
+    </row>
+    <row r="17" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="86"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="85"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="68"/>
+    </row>
+    <row r="18" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="68"/>
+    </row>
+    <row r="19" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
+    </row>
+    <row r="20" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="69"/>
+      <c r="H20" s="69"/>
+    </row>
+    <row r="21" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="69"/>
+    </row>
+    <row r="22" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="69"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="69"/>
+      <c r="J22" s="69"/>
+      <c r="K22" s="69"/>
+    </row>
+    <row r="23" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="69"/>
+      <c r="H23" s="69"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="69"/>
+    </row>
+    <row r="24" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+    </row>
+    <row r="25" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="69"/>
+      <c r="H25" s="69"/>
+      <c r="I25" s="69"/>
+      <c r="J25" s="69"/>
+      <c r="K25" s="69"/>
+    </row>
+    <row r="26" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="69"/>
+      <c r="H26" s="69"/>
+      <c r="I26" s="69"/>
+      <c r="J26" s="69"/>
+      <c r="K26" s="69"/>
+    </row>
+    <row r="27" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G27" s="69"/>
+      <c r="H27" s="69"/>
+      <c r="I27" s="69"/>
+      <c r="J27" s="69"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="69"/>
+      <c r="H28" s="69"/>
+      <c r="I28" s="69"/>
+      <c r="J28" s="69"/>
+      <c r="K28" s="69"/>
+    </row>
+    <row r="29" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="69"/>
+      <c r="H29" s="69"/>
+      <c r="I29" s="69"/>
+      <c r="J29" s="69"/>
+      <c r="K29" s="69"/>
+    </row>
+    <row r="30" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G30" s="69"/>
+      <c r="H30" s="69"/>
+    </row>
+    <row r="31" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G31" s="69"/>
+      <c r="H31" s="69"/>
+    </row>
+    <row r="32" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G32" s="69"/>
+      <c r="H32" s="69"/>
+    </row>
+    <row r="33" spans="7:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
+    </row>
+    <row r="34" spans="7:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+    </row>
+    <row r="35" spans="7:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G35" s="69"/>
+      <c r="H35" s="69"/>
+    </row>
+    <row r="36" spans="7:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G36" s="69"/>
+      <c r="H36" s="69"/>
+    </row>
+    <row r="37" spans="7:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G37" s="69"/>
+      <c r="H37" s="69"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="E4:E8"/>
+    <mergeCell ref="F4:F8"/>
+    <mergeCell ref="G4:G8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86259380-E3BB-4E8B-A780-CD8F388C7A70}">
+  <dimension ref="A1:K31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="26.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="19.140625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="11.42578125" style="1"/>
@@ -8593,68 +9388,82 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71"/>
-      <c r="B4" s="183" t="s">
-        <v>125</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="127" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="127"/>
-      <c r="F4" s="127"/>
-      <c r="G4" s="156"/>
-      <c r="H4" s="129" t="s">
+      <c r="B4" s="227" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="239" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="242" t="s">
         <v>75</v>
       </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
-      <c r="B5" s="183" t="s">
-        <v>126</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="127" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="127"/>
-      <c r="F5" s="127"/>
-      <c r="G5" s="156"/>
-      <c r="H5" s="129" t="s">
-        <v>75</v>
-      </c>
+      <c r="B5" s="229"/>
+      <c r="C5" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="240"/>
+      <c r="H5" s="243"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="71"/>
-      <c r="B6" s="183" t="s">
-        <v>127</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="127" t="s">
-        <v>124</v>
-      </c>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="128" t="s">
+      <c r="B6" s="229"/>
+      <c r="C6" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="241"/>
+      <c r="H6" s="244"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="71"/>
+      <c r="B7" s="188" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="245" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="129" t="s">
-        <v>75</v>
-      </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="71"/>
-      <c r="B7" s="183"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="127"/>
-      <c r="E7" s="127"/>
-      <c r="F7" s="127"/>
-      <c r="G7" s="156"/>
-      <c r="H7" s="129" t="s">
+      <c r="H7" s="187" t="s">
         <v>75</v>
       </c>
       <c r="I7" s="3"/>
@@ -8664,41 +9473,41 @@
       <c r="B8" s="150" t="s">
         <v>119</v>
       </c>
-      <c r="C8" s="151" t="s">
+      <c r="C8" s="197" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="149" t="s">
+      <c r="D8" s="199" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="149" t="s">
+      <c r="E8" s="199" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="149" t="s">
+      <c r="F8" s="199" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="218" t="s">
+      <c r="G8" s="237" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="219"/>
+      <c r="H8" s="235"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="71"/>
       <c r="B9" s="153" t="s">
         <v>92</v>
       </c>
       <c r="C9" s="154"/>
-      <c r="D9" s="155" t="s">
+      <c r="D9" s="198" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="155" t="s">
+      <c r="E9" s="198" t="s">
         <v>71</v>
       </c>
-      <c r="F9" s="155"/>
-      <c r="G9" s="201" t="s">
+      <c r="F9" s="198"/>
+      <c r="G9" s="217" t="s">
         <v>75</v>
       </c>
-      <c r="H9" s="202"/>
+      <c r="H9" s="218"/>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -8828,12 +9637,15 @@
       <c r="H31" s="69"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9019,15 +9831,15 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50F9D30A-50A2-408B-B3F0-EDB4CF8C0B75}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="9261f3b7-eb37-44bc-ab49-41e0f5c5a530"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="9261f3b7-eb37-44bc-ab49-41e0f5c5a530"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
KW 15 File Upload
</commit_message>
<xml_diff>
--- a/website/src/documents/allgemein/Apollon_Projektplan.xlsx
+++ b/website/src/documents/allgemein/Apollon_Projektplan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dhbwstg.sharepoint.com/sites/o365grpSWE-Projekt/Freigegebene Dokumente/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="803" documentId="8_{45909616-94BE-491C-BFA5-6DC92E6FFB12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A756FFEA-6DD9-4D3A-9D01-8D9897A5F3EB}"/>
+  <xr:revisionPtr revIDLastSave="871" documentId="8_{45909616-94BE-491C-BFA5-6DC92E6FFB12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CAC862D9-C6D2-4C2D-A167-D3E6B2BA4539}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="8" xr2:uid="{5DFA726E-B0C4-4500-AF96-5BC0FDCBA0B9}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="171">
   <si>
     <r>
       <t xml:space="preserve">Zielsetzung
@@ -571,16 +571,64 @@
     <t>Design Beschreibung</t>
   </si>
   <si>
-    <t>Implementieren des Endprodukts</t>
-  </si>
-  <si>
-    <t>Planung noch nicht vollständig abgeschlossen</t>
-  </si>
-  <si>
     <t>5h</t>
   </si>
   <si>
-    <t>-</t>
+    <t>35h</t>
+  </si>
+  <si>
+    <t>Implementieren des Backends</t>
+  </si>
+  <si>
+    <t>Implementieren der DTOs</t>
+  </si>
+  <si>
+    <t>Implemetieren des Frontends</t>
+  </si>
+  <si>
+    <t>Implementieren der Razor Components</t>
+  </si>
+  <si>
+    <t>Implementieren der Services</t>
+  </si>
+  <si>
+    <t>Implementieren der Service-Klassen</t>
+  </si>
+  <si>
+    <t>Implementieren der Modell-Klassen und Datenanbindung</t>
+  </si>
+  <si>
+    <t>Implementieren der REST-Schnittstellen</t>
+  </si>
+  <si>
+    <t>Implementieren der SignalR-Schnittstellen</t>
+  </si>
+  <si>
+    <t>15h</t>
+  </si>
+  <si>
+    <t>50h</t>
+  </si>
+  <si>
+    <t>Erster Schritt</t>
+  </si>
+  <si>
+    <t>70h</t>
+  </si>
+  <si>
+    <t>Top-Down Implementierung</t>
+  </si>
+  <si>
+    <t>Bottom-up Implementierung</t>
+  </si>
+  <si>
+    <t>60h</t>
+  </si>
+  <si>
+    <t>Wöchentlich</t>
+  </si>
+  <si>
+    <t>Wöchentlich Updaten</t>
   </si>
 </sst>
 </file>
@@ -2311,7 +2359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="248">
+  <cellXfs count="252">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2896,6 +2944,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4913,11 +4973,11 @@
     </row>
     <row r="3" spans="1:15" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
-      <c r="B3" s="203" t="s">
+      <c r="B3" s="207" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="204"/>
-      <c r="D3" s="205"/>
+      <c r="C3" s="208"/>
+      <c r="D3" s="209"/>
       <c r="E3" s="101"/>
       <c r="F3" s="101"/>
       <c r="G3" s="101"/>
@@ -4932,11 +4992,11 @@
     </row>
     <row r="4" spans="1:15" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="112"/>
-      <c r="B4" s="206" t="s">
+      <c r="B4" s="210" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="207"/>
-      <c r="D4" s="208"/>
+      <c r="C4" s="211"/>
+      <c r="D4" s="212"/>
       <c r="E4" s="103"/>
       <c r="F4" s="103"/>
       <c r="G4" s="103"/>
@@ -4951,9 +5011,9 @@
     </row>
     <row r="5" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="112"/>
-      <c r="B5" s="209"/>
-      <c r="C5" s="210"/>
-      <c r="D5" s="211"/>
+      <c r="B5" s="213"/>
+      <c r="C5" s="214"/>
+      <c r="D5" s="215"/>
       <c r="E5" s="103"/>
       <c r="F5" s="103"/>
       <c r="G5" s="103"/>
@@ -4968,9 +5028,9 @@
     </row>
     <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="112"/>
-      <c r="B6" s="209"/>
-      <c r="C6" s="210"/>
-      <c r="D6" s="211"/>
+      <c r="B6" s="213"/>
+      <c r="C6" s="214"/>
+      <c r="D6" s="215"/>
       <c r="E6" s="103"/>
       <c r="F6" s="103"/>
       <c r="G6" s="103"/>
@@ -4985,9 +5045,9 @@
     </row>
     <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="112"/>
-      <c r="B7" s="209"/>
-      <c r="C7" s="210"/>
-      <c r="D7" s="211"/>
+      <c r="B7" s="213"/>
+      <c r="C7" s="214"/>
+      <c r="D7" s="215"/>
       <c r="E7" s="103"/>
       <c r="F7" s="103"/>
       <c r="G7" s="103"/>
@@ -5002,9 +5062,9 @@
     </row>
     <row r="8" spans="1:15" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="112"/>
-      <c r="B8" s="209"/>
-      <c r="C8" s="210"/>
-      <c r="D8" s="211"/>
+      <c r="B8" s="213"/>
+      <c r="C8" s="214"/>
+      <c r="D8" s="215"/>
       <c r="E8" s="103"/>
       <c r="F8" s="103"/>
       <c r="G8" s="103"/>
@@ -5019,9 +5079,9 @@
     </row>
     <row r="9" spans="1:15" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="112"/>
-      <c r="B9" s="212"/>
-      <c r="C9" s="213"/>
-      <c r="D9" s="214"/>
+      <c r="B9" s="216"/>
+      <c r="C9" s="217"/>
+      <c r="D9" s="218"/>
       <c r="E9" s="103"/>
       <c r="F9" s="103"/>
       <c r="G9" s="103"/>
@@ -6029,10 +6089,10 @@
     <row r="4" spans="1:13" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="157"/>
       <c r="E4" s="156"/>
-      <c r="F4" s="215" t="s">
+      <c r="F4" s="219" t="s">
         <v>99</v>
       </c>
-      <c r="G4" s="216"/>
+      <c r="G4" s="220"/>
       <c r="H4" s="178"/>
       <c r="I4" s="157"/>
       <c r="J4" s="157"/>
@@ -6071,11 +6131,11 @@
         <v>100</v>
       </c>
       <c r="C7" s="146"/>
-      <c r="D7" s="217" t="s">
+      <c r="D7" s="221" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="218"/>
-      <c r="F7" s="219"/>
+      <c r="E7" s="222"/>
+      <c r="F7" s="223"/>
       <c r="G7" s="146"/>
       <c r="H7" s="145" t="s">
         <v>102</v>
@@ -8253,7 +8313,7 @@
     </row>
     <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71"/>
-      <c r="B4" s="224" t="s">
+      <c r="B4" s="228" t="s">
         <v>58</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -8262,48 +8322,48 @@
       <c r="D4" s="123" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="227" t="s">
+      <c r="E4" s="231" t="s">
         <v>61</v>
       </c>
       <c r="F4" s="123"/>
-      <c r="G4" s="228" t="s">
+      <c r="G4" s="232" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="229" t="s">
+      <c r="H4" s="233" t="s">
         <v>62</v>
       </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
-      <c r="B5" s="225"/>
+      <c r="B5" s="229"/>
       <c r="C5" s="7" t="s">
         <v>63</v>
       </c>
       <c r="D5" s="123" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="227"/>
+      <c r="E5" s="231"/>
       <c r="F5" s="123"/>
-      <c r="G5" s="228"/>
-      <c r="H5" s="229"/>
+      <c r="G5" s="232"/>
+      <c r="H5" s="233"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="71"/>
-      <c r="B6" s="226"/>
+      <c r="B6" s="230"/>
       <c r="C6" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D6" s="123" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="227"/>
+      <c r="E6" s="231"/>
       <c r="F6" s="123" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="228"/>
-      <c r="H6" s="229"/>
+      <c r="G6" s="232"/>
+      <c r="H6" s="233"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8396,13 +8456,13 @@
     </row>
     <row r="11" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="71"/>
-      <c r="B11" s="230" t="s">
+      <c r="B11" s="234" t="s">
         <v>84</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="234" t="s">
+      <c r="D11" s="238" t="s">
         <v>73</v>
       </c>
       <c r="E11" s="127" t="s">
@@ -8419,11 +8479,11 @@
     </row>
     <row r="12" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="71"/>
-      <c r="B12" s="232"/>
+      <c r="B12" s="236"/>
       <c r="C12" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="235"/>
+      <c r="D12" s="239"/>
       <c r="E12" s="127" t="s">
         <v>69</v>
       </c>
@@ -8438,11 +8498,11 @@
     </row>
     <row r="13" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="71"/>
-      <c r="B13" s="233"/>
+      <c r="B13" s="237"/>
       <c r="C13" s="127" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="236"/>
+      <c r="D13" s="240"/>
       <c r="E13" s="127" t="s">
         <v>89</v>
       </c>
@@ -8472,14 +8532,14 @@
       <c r="F14" s="149" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="237" t="s">
+      <c r="G14" s="241" t="s">
         <v>57</v>
       </c>
-      <c r="H14" s="238"/>
+      <c r="H14" s="242"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="230" t="s">
+      <c r="B15" s="234" t="s">
         <v>77</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -8494,13 +8554,13 @@
       <c r="F15" s="123" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="222" t="s">
+      <c r="G15" s="226" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="223"/>
+      <c r="H15" s="227"/>
     </row>
     <row r="16" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="231"/>
+      <c r="B16" s="235"/>
       <c r="C16" s="7" t="s">
         <v>82</v>
       </c>
@@ -8511,10 +8571,10 @@
         <v>83</v>
       </c>
       <c r="F16" s="123"/>
-      <c r="G16" s="222" t="s">
+      <c r="G16" s="226" t="s">
         <v>62</v>
       </c>
-      <c r="H16" s="223"/>
+      <c r="H16" s="227"/>
     </row>
     <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="153" t="s">
@@ -8528,10 +8588,10 @@
         <v>71</v>
       </c>
       <c r="F17" s="155"/>
-      <c r="G17" s="220" t="s">
+      <c r="G17" s="224" t="s">
         <v>75</v>
       </c>
-      <c r="H17" s="221"/>
+      <c r="H17" s="225"/>
     </row>
     <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
@@ -8695,7 +8755,7 @@
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="71"/>
-      <c r="B4" s="239" t="s">
+      <c r="B4" s="243" t="s">
         <v>90</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -8706,7 +8766,7 @@
       </c>
       <c r="E4" s="123"/>
       <c r="F4" s="123"/>
-      <c r="G4" s="228" t="s">
+      <c r="G4" s="232" t="s">
         <v>62</v>
       </c>
       <c r="H4" s="180" t="s">
@@ -8716,7 +8776,7 @@
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
-      <c r="B5" s="239"/>
+      <c r="B5" s="243"/>
       <c r="C5" s="7" t="s">
         <v>122</v>
       </c>
@@ -8725,7 +8785,7 @@
       </c>
       <c r="E5" s="123"/>
       <c r="F5" s="123"/>
-      <c r="G5" s="228"/>
+      <c r="G5" s="232"/>
       <c r="H5" s="180" t="s">
         <v>62</v>
       </c>
@@ -8733,7 +8793,7 @@
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="71"/>
-      <c r="B6" s="239"/>
+      <c r="B6" s="243"/>
       <c r="C6" s="7" t="s">
         <v>123</v>
       </c>
@@ -8742,7 +8802,7 @@
       </c>
       <c r="E6" s="123"/>
       <c r="F6" s="123"/>
-      <c r="G6" s="228"/>
+      <c r="G6" s="232"/>
       <c r="H6" s="180" t="s">
         <v>62</v>
       </c>
@@ -8750,7 +8810,7 @@
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="71"/>
-      <c r="B7" s="239"/>
+      <c r="B7" s="243"/>
       <c r="C7" s="7" t="s">
         <v>91</v>
       </c>
@@ -8759,7 +8819,7 @@
       </c>
       <c r="E7" s="123"/>
       <c r="F7" s="123"/>
-      <c r="G7" s="228"/>
+      <c r="G7" s="232"/>
       <c r="H7" s="180" t="s">
         <v>62</v>
       </c>
@@ -8782,10 +8842,10 @@
       <c r="F8" s="149" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="237" t="s">
+      <c r="G8" s="241" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="238"/>
+      <c r="H8" s="242"/>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8801,10 +8861,10 @@
         <v>71</v>
       </c>
       <c r="F9" s="155"/>
-      <c r="G9" s="220" t="s">
+      <c r="G9" s="224" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="221"/>
+      <c r="H9" s="225"/>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -8988,22 +9048,22 @@
     </row>
     <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="71"/>
-      <c r="B4" s="230" t="s">
+      <c r="B4" s="234" t="s">
         <v>125</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D4" s="234" t="s">
+      <c r="D4" s="238" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="234" t="s">
+      <c r="E4" s="238" t="s">
         <v>141</v>
       </c>
-      <c r="F4" s="234" t="s">
+      <c r="F4" s="238" t="s">
         <v>139</v>
       </c>
-      <c r="G4" s="242" t="s">
+      <c r="G4" s="246" t="s">
         <v>62</v>
       </c>
       <c r="H4" s="200" t="s">
@@ -9013,14 +9073,14 @@
     </row>
     <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
-      <c r="B5" s="232"/>
+      <c r="B5" s="236"/>
       <c r="C5" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D5" s="235"/>
-      <c r="E5" s="235"/>
-      <c r="F5" s="235"/>
-      <c r="G5" s="243"/>
+      <c r="D5" s="239"/>
+      <c r="E5" s="239"/>
+      <c r="F5" s="239"/>
+      <c r="G5" s="247"/>
       <c r="H5" s="200" t="s">
         <v>62</v>
       </c>
@@ -9028,14 +9088,14 @@
     </row>
     <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="71"/>
-      <c r="B6" s="232"/>
+      <c r="B6" s="236"/>
       <c r="C6" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="235"/>
-      <c r="E6" s="235"/>
-      <c r="F6" s="235"/>
-      <c r="G6" s="243"/>
+      <c r="D6" s="239"/>
+      <c r="E6" s="239"/>
+      <c r="F6" s="239"/>
+      <c r="G6" s="247"/>
       <c r="H6" s="200" t="s">
         <v>62</v>
       </c>
@@ -9043,14 +9103,14 @@
     </row>
     <row r="7" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="71"/>
-      <c r="B7" s="232"/>
+      <c r="B7" s="236"/>
       <c r="C7" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D7" s="235"/>
-      <c r="E7" s="235"/>
-      <c r="F7" s="235"/>
-      <c r="G7" s="243"/>
+      <c r="D7" s="239"/>
+      <c r="E7" s="239"/>
+      <c r="F7" s="239"/>
+      <c r="G7" s="247"/>
       <c r="H7" s="200" t="s">
         <v>62</v>
       </c>
@@ -9058,14 +9118,14 @@
     </row>
     <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="71"/>
-      <c r="B8" s="231"/>
+      <c r="B8" s="235"/>
       <c r="C8" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D8" s="241"/>
-      <c r="E8" s="241"/>
-      <c r="F8" s="241"/>
-      <c r="G8" s="244"/>
+      <c r="D8" s="245"/>
+      <c r="E8" s="245"/>
+      <c r="F8" s="245"/>
+      <c r="G8" s="248"/>
       <c r="H8" s="200" t="s">
         <v>62</v>
       </c>
@@ -9191,10 +9251,10 @@
       <c r="F14" s="197" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="240" t="s">
+      <c r="G14" s="244" t="s">
         <v>57</v>
       </c>
-      <c r="H14" s="238"/>
+      <c r="H14" s="242"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -9210,10 +9270,10 @@
         <v>71</v>
       </c>
       <c r="F15" s="196"/>
-      <c r="G15" s="220" t="s">
+      <c r="G15" s="224" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="221"/>
+      <c r="H15" s="225"/>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9362,7 +9422,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9427,7 +9487,7 @@
     </row>
     <row r="4" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71"/>
-      <c r="B4" s="230" t="s">
+      <c r="B4" s="234" t="s">
         <v>114</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -9440,17 +9500,17 @@
         <v>147</v>
       </c>
       <c r="F4" s="7"/>
-      <c r="G4" s="242" t="s">
+      <c r="G4" s="246" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="245" t="s">
+      <c r="H4" s="249" t="s">
         <v>62</v>
       </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
-      <c r="B5" s="232"/>
+      <c r="B5" s="236"/>
       <c r="C5" s="7" t="s">
         <v>144</v>
       </c>
@@ -9461,13 +9521,13 @@
         <v>80</v>
       </c>
       <c r="F5" s="7"/>
-      <c r="G5" s="243"/>
-      <c r="H5" s="246"/>
+      <c r="G5" s="247"/>
+      <c r="H5" s="250"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="71"/>
-      <c r="B6" s="232"/>
+      <c r="B6" s="236"/>
       <c r="C6" s="7" t="s">
         <v>145</v>
       </c>
@@ -9478,8 +9538,8 @@
         <v>80</v>
       </c>
       <c r="F6" s="7"/>
-      <c r="G6" s="244"/>
-      <c r="H6" s="247"/>
+      <c r="G6" s="248"/>
+      <c r="H6" s="251"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -9522,10 +9582,10 @@
       <c r="F8" s="197" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="240" t="s">
+      <c r="G8" s="244" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="238"/>
+      <c r="H8" s="242"/>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -9541,10 +9601,10 @@
         <v>71</v>
       </c>
       <c r="F9" s="196"/>
-      <c r="G9" s="220" t="s">
+      <c r="G9" s="224" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="221"/>
+      <c r="H9" s="225"/>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9688,16 +9748,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCE834A-8DD0-4885-B464-1A119C3BFD73}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="26.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="42.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="34.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -9756,20 +9816,20 @@
     </row>
     <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="71"/>
-      <c r="B4" s="230" t="s">
-        <v>151</v>
+      <c r="B4" s="206" t="s">
+        <v>154</v>
       </c>
       <c r="C4" s="7"/>
-      <c r="D4" s="234" t="s">
+      <c r="D4" s="238" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="234" t="s">
-        <v>154</v>
-      </c>
-      <c r="F4" s="234" t="s">
-        <v>152</v>
-      </c>
-      <c r="G4" s="242" t="s">
+      <c r="E4" s="204" t="s">
+        <v>162</v>
+      </c>
+      <c r="F4" s="204" t="s">
+        <v>164</v>
+      </c>
+      <c r="G4" s="246" t="s">
         <v>75</v>
       </c>
       <c r="H4" s="201" t="s">
@@ -9779,25 +9839,37 @@
     </row>
     <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
-      <c r="B5" s="232"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="235"/>
-      <c r="E5" s="235"/>
-      <c r="F5" s="235"/>
-      <c r="G5" s="243"/>
-      <c r="H5" s="201" t="s">
+      <c r="B5" s="234" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="239"/>
+      <c r="E5" s="205" t="s">
+        <v>163</v>
+      </c>
+      <c r="F5" s="239" t="s">
+        <v>166</v>
+      </c>
+      <c r="G5" s="247"/>
+      <c r="H5" s="203" t="s">
         <v>75</v>
       </c>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="71"/>
-      <c r="B6" s="232"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="235"/>
-      <c r="E6" s="235"/>
-      <c r="F6" s="235"/>
-      <c r="G6" s="243"/>
+      <c r="B6" s="236"/>
+      <c r="C6" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="239"/>
+      <c r="E6" s="205" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="239"/>
+      <c r="G6" s="247"/>
       <c r="H6" s="201" t="s">
         <v>75</v>
       </c>
@@ -9805,229 +9877,284 @@
     </row>
     <row r="7" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="71"/>
-      <c r="B7" s="232"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="235"/>
-      <c r="E7" s="235"/>
-      <c r="F7" s="235"/>
-      <c r="G7" s="243"/>
-      <c r="H7" s="201" t="s">
+      <c r="B7" s="235"/>
+      <c r="C7" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" s="239"/>
+      <c r="E7" s="205" t="s">
+        <v>151</v>
+      </c>
+      <c r="F7" s="239"/>
+      <c r="G7" s="247"/>
+      <c r="H7" s="203" t="s">
         <v>75</v>
       </c>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="71"/>
-      <c r="B8" s="231"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="241"/>
-      <c r="E8" s="241"/>
-      <c r="F8" s="241"/>
-      <c r="G8" s="244"/>
-      <c r="H8" s="201" t="s">
+      <c r="B8" s="234" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D8" s="239"/>
+      <c r="E8" s="205" t="s">
+        <v>165</v>
+      </c>
+      <c r="F8" s="239" t="s">
+        <v>167</v>
+      </c>
+      <c r="G8" s="247"/>
+      <c r="H8" s="203" t="s">
         <v>75</v>
       </c>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="71"/>
-      <c r="B9" s="202" t="s">
+      <c r="B9" s="236"/>
+      <c r="C9" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D9" s="239"/>
+      <c r="E9" s="205" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" s="239"/>
+      <c r="G9" s="247"/>
+      <c r="H9" s="203" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="71"/>
+      <c r="B10" s="236"/>
+      <c r="C10" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" s="239"/>
+      <c r="E10" s="205" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="239"/>
+      <c r="G10" s="247"/>
+      <c r="H10" s="203" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="71"/>
+      <c r="B11" s="235"/>
+      <c r="C11" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" s="239"/>
+      <c r="E11" s="205" t="s">
+        <v>168</v>
+      </c>
+      <c r="F11" s="245"/>
+      <c r="G11" s="247"/>
+      <c r="H11" s="201" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="71"/>
+      <c r="B12" s="202" t="s">
         <v>148</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="199" t="s">
+      <c r="C12" s="7"/>
+      <c r="D12" s="199" t="s">
         <v>149</v>
       </c>
-      <c r="E9" s="199" t="s">
+      <c r="E12" s="199" t="s">
         <v>129</v>
       </c>
-      <c r="F9" s="199"/>
-      <c r="G9" s="200" t="s">
+      <c r="F12" s="199"/>
+      <c r="G12" s="200" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="201" t="s">
+      <c r="H12" s="201" t="s">
         <v>75</v>
       </c>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="71"/>
-      <c r="B10" s="202" t="s">
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="71"/>
+      <c r="B13" s="202" t="s">
         <v>150</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="199" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="199" t="s">
         <v>140</v>
       </c>
-      <c r="E10" s="199" t="s">
-        <v>153</v>
-      </c>
-      <c r="F10" s="199"/>
-      <c r="G10" s="200" t="s">
+      <c r="E13" s="199" t="s">
+        <v>152</v>
+      </c>
+      <c r="F13" s="199" t="s">
+        <v>170</v>
+      </c>
+      <c r="G13" s="200" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="201" t="s">
+      <c r="H13" s="201" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="71"/>
-      <c r="B11" s="150" t="s">
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="71"/>
+      <c r="B14" s="150" t="s">
         <v>119</v>
       </c>
-      <c r="C11" s="195" t="s">
+      <c r="C14" s="195" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="197" t="s">
+      <c r="D14" s="197" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="197" t="s">
+      <c r="E14" s="197" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="197" t="s">
+      <c r="F14" s="197" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="240" t="s">
+      <c r="G14" s="244" t="s">
         <v>57</v>
       </c>
-      <c r="H11" s="238"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="71"/>
-      <c r="B12" s="153" t="s">
+      <c r="H14" s="242"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="71"/>
+      <c r="B15" s="153" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="154"/>
-      <c r="D12" s="196" t="s">
+      <c r="C15" s="154"/>
+      <c r="D15" s="196" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="196" t="s">
+      <c r="E15" s="196" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="196"/>
-      <c r="G12" s="220" t="s">
+      <c r="F15" s="196" t="s">
+        <v>169</v>
+      </c>
+      <c r="G15" s="224" t="s">
         <v>75</v>
       </c>
-      <c r="H12" s="221"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="87"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="89"/>
-      <c r="H13" s="74"/>
-    </row>
-    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="86"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="85"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="68"/>
-    </row>
-    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="66"/>
-      <c r="D15" s="66"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="68"/>
+      <c r="H15" s="225"/>
+      <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G16" s="69"/>
-      <c r="H16" s="69"/>
-    </row>
-    <row r="17" spans="7:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G17" s="69"/>
-      <c r="H17" s="69"/>
-    </row>
-    <row r="18" spans="7:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="87"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="89"/>
+      <c r="H16" s="74"/>
+    </row>
+    <row r="17" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="86"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="85"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="68"/>
+    </row>
+    <row r="18" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
       <c r="G18" s="69"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
-      <c r="K18" s="69"/>
-    </row>
-    <row r="19" spans="7:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="68"/>
+    </row>
+    <row r="19" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G19" s="69"/>
       <c r="H19" s="69"/>
-      <c r="I19" s="69"/>
-      <c r="J19" s="69"/>
-      <c r="K19" s="69"/>
-    </row>
-    <row r="20" spans="7:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G20" s="69"/>
       <c r="H20" s="69"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="69"/>
-    </row>
-    <row r="21" spans="7:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G21" s="69"/>
       <c r="H21" s="69"/>
       <c r="I21" s="69"/>
       <c r="J21" s="69"/>
       <c r="K21" s="69"/>
     </row>
-    <row r="22" spans="7:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G22" s="69"/>
       <c r="H22" s="69"/>
       <c r="I22" s="69"/>
       <c r="J22" s="69"/>
       <c r="K22" s="69"/>
     </row>
-    <row r="23" spans="7:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G23" s="69"/>
       <c r="H23" s="69"/>
       <c r="I23" s="69"/>
       <c r="J23" s="69"/>
       <c r="K23" s="69"/>
     </row>
-    <row r="24" spans="7:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G24" s="69"/>
       <c r="H24" s="69"/>
       <c r="I24" s="69"/>
       <c r="J24" s="69"/>
       <c r="K24" s="69"/>
     </row>
-    <row r="25" spans="7:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G25" s="69"/>
       <c r="H25" s="69"/>
       <c r="I25" s="69"/>
       <c r="J25" s="69"/>
       <c r="K25" s="69"/>
     </row>
-    <row r="26" spans="7:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G26" s="69"/>
       <c r="H26" s="69"/>
       <c r="I26" s="69"/>
       <c r="J26" s="69"/>
       <c r="K26" s="69"/>
     </row>
-    <row r="27" spans="7:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G27" s="69"/>
       <c r="H27" s="69"/>
-    </row>
-    <row r="28" spans="7:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I27" s="69"/>
+      <c r="J27" s="69"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G28" s="69"/>
       <c r="H28" s="69"/>
-    </row>
-    <row r="29" spans="7:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I28" s="69"/>
+      <c r="J28" s="69"/>
+      <c r="K28" s="69"/>
+    </row>
+    <row r="29" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G29" s="69"/>
       <c r="H29" s="69"/>
-    </row>
-    <row r="30" spans="7:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="69"/>
+      <c r="J29" s="69"/>
+      <c r="K29" s="69"/>
+    </row>
+    <row r="30" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G30" s="69"/>
       <c r="H30" s="69"/>
     </row>
-    <row r="31" spans="7:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G31" s="69"/>
       <c r="H31" s="69"/>
     </row>
-    <row r="32" spans="7:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G32" s="69"/>
       <c r="H32" s="69"/>
     </row>
@@ -10039,15 +10166,28 @@
       <c r="G34" s="69"/>
       <c r="H34" s="69"/>
     </row>
+    <row r="35" spans="7:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G35" s="69"/>
+      <c r="H35" s="69"/>
+    </row>
+    <row r="36" spans="7:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G36" s="69"/>
+      <c r="H36" s="69"/>
+    </row>
+    <row r="37" spans="7:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G37" s="69"/>
+      <c r="H37" s="69"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="E4:E8"/>
-    <mergeCell ref="F4:F8"/>
-    <mergeCell ref="G4:G8"/>
-    <mergeCell ref="G11:H11"/>
+  <mergeCells count="8">
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="D4:D11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="G14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10219,18 +10359,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10252,25 +10392,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50F9D30A-50A2-408B-B3F0-EDB4CF8C0B75}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFCF450D-C3EB-4368-8E96-CCC92F1AC82B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9261f3b7-eb37-44bc-ab49-41e0f5c5a530"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFCF450D-C3EB-4368-8E96-CCC92F1AC82B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50F9D30A-50A2-408B-B3F0-EDB4CF8C0B75}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9261f3b7-eb37-44bc-ab49-41e0f5c5a530"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Uploaded Files for KW17
</commit_message>
<xml_diff>
--- a/website/src/documents/allgemein/Apollon_Projektplan.xlsx
+++ b/website/src/documents/allgemein/Apollon_Projektplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dhbwstg.sharepoint.com/sites/o365grpSWE-Projekt/Freigegebene Dokumente/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="871" documentId="8_{45909616-94BE-491C-BFA5-6DC92E6FFB12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CAC862D9-C6D2-4C2D-A167-D3E6B2BA4539}"/>
+  <xr:revisionPtr revIDLastSave="878" documentId="8_{45909616-94BE-491C-BFA5-6DC92E6FFB12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CEF06606-73D3-42D1-BEB9-CBBC7A87EBE5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="8" xr2:uid="{5DFA726E-B0C4-4500-AF96-5BC0FDCBA0B9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="8" xr2:uid="{5DFA726E-B0C4-4500-AF96-5BC0FDCBA0B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Zielsetzung" sheetId="5" r:id="rId1"/>
@@ -171,215 +171,28 @@
     <t>Abgabetermine</t>
   </si>
   <si>
+    <t>Aufgabenblatt 1</t>
+  </si>
+  <si>
+    <t>Aufgabenblatt 2</t>
+  </si>
+  <si>
+    <t>Aufgabenblatt 3</t>
+  </si>
+  <si>
+    <t>Aufgabenblatt 4</t>
+  </si>
+  <si>
+    <t>Aufgabenblatt 5</t>
+  </si>
+  <si>
+    <t>Aufgabenblatt 6</t>
+  </si>
+  <si>
     <t>Sonstiges Termine</t>
   </si>
   <si>
     <t>Archivdatei</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Mitglied
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Castellar"/>
-      </rPr>
-      <t>Apollon</t>
-    </r>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Rolle</t>
-  </si>
-  <si>
-    <t>Stellvertretend</t>
-  </si>
-  <si>
-    <t>Florian Albert</t>
-  </si>
-  <si>
-    <t>Verantwortlicher für Implementierung</t>
-  </si>
-  <si>
-    <t>Projektleiter</t>
-  </si>
-  <si>
-    <t>Paul-Benedict Burkard</t>
-  </si>
-  <si>
-    <t>Leon Jerke</t>
-  </si>
-  <si>
-    <t>Verantwortlicher für Tests</t>
-  </si>
-  <si>
-    <t>Technischer Assistent / Verantwortlicher für Modellierung</t>
-  </si>
-  <si>
-    <t>Daniel Kröker</t>
-  </si>
-  <si>
-    <t>Qualitätssicherung und Dokumentation</t>
-  </si>
-  <si>
-    <t>Verantwortlicher für Recherche</t>
-  </si>
-  <si>
-    <t>Alfred Rustemi</t>
-  </si>
-  <si>
-    <t>Etienne Zink</t>
-  </si>
-  <si>
-    <t>Gefordertes Artefakt</t>
-  </si>
-  <si>
-    <t>Meilensteine</t>
-  </si>
-  <si>
-    <t>Verantwortlich</t>
-  </si>
-  <si>
-    <t>Geschätzter Aufwand</t>
-  </si>
-  <si>
-    <t>Anmerkungen</t>
-  </si>
-  <si>
-    <t>Hochladen?</t>
-  </si>
-  <si>
-    <t>Fertigsgestellt</t>
-  </si>
-  <si>
-    <t>Projektplan</t>
-  </si>
-  <si>
-    <t>Aufsetzen des Projektplans</t>
-  </si>
-  <si>
-    <t>Projektleiter | Paul-Benedict Burkard</t>
-  </si>
-  <si>
-    <t>8h</t>
-  </si>
-  <si>
-    <t>ü</t>
-  </si>
-  <si>
-    <t>Besprechen der Elemente mit dem Team</t>
-  </si>
-  <si>
-    <t>Gesamtes Team</t>
-  </si>
-  <si>
-    <t>Pflegen des Projektplans</t>
-  </si>
-  <si>
-    <t>Kontinuierliche Aufgabe, nicht auf dieses Blatt begrenzt</t>
-  </si>
-  <si>
-    <t>Risikoanalyse</t>
-  </si>
-  <si>
-    <t>Verantwortlicher für Qualitätssicherung | Daniel Kröker</t>
-  </si>
-  <si>
-    <t>1h</t>
-  </si>
-  <si>
-    <t>Rollenverteilung</t>
-  </si>
-  <si>
-    <t>30min</t>
-  </si>
-  <si>
-    <t>IDE/UML-Werkzeuge</t>
-  </si>
-  <si>
-    <t>Technischer Assistent | Etienne Zink</t>
-  </si>
-  <si>
-    <t>Mit Betreuer abzusprechen</t>
-  </si>
-  <si>
-    <t>û</t>
-  </si>
-  <si>
-    <t>GIT-Entscheidung</t>
-  </si>
-  <si>
-    <t>SCRUM Dokumentation</t>
-  </si>
-  <si>
-    <t>SCRUM einrichten</t>
-  </si>
-  <si>
-    <t>Verantwortlicher für Implementierung | Florian Albert</t>
-  </si>
-  <si>
-    <t>2h</t>
-  </si>
-  <si>
-    <t>Gehosted auf GitHub</t>
-  </si>
-  <si>
-    <t>Dokumentation veröffentlichen</t>
-  </si>
-  <si>
-    <t>30h</t>
-  </si>
-  <si>
-    <t>Gruppen Homepage</t>
-  </si>
-  <si>
-    <t>Aufsetzen der Homepage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Website erstellen: Leon 
-Server hosten: Etienne </t>
-  </si>
-  <si>
-    <t>Tutorial für das Team</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hochladen aller Artefakte </t>
-  </si>
-  <si>
-    <t>15min</t>
-  </si>
-  <si>
-    <t>Recherchebericht</t>
-  </si>
-  <si>
-    <t>Formulierung des Berichts</t>
-  </si>
-  <si>
-    <t>Aufwandsbericht</t>
-  </si>
-  <si>
-    <t>Aufgabenblatt 1</t>
-  </si>
-  <si>
-    <t>Aufgabenblatt 2</t>
-  </si>
-  <si>
-    <t>Aufgabenblatt 3</t>
-  </si>
-  <si>
-    <t>Aufgabenblatt 4</t>
-  </si>
-  <si>
-    <t>Aufgabenblatt 5</t>
-  </si>
-  <si>
-    <t>Aufgabenblatt 6</t>
   </si>
   <si>
     <r>
@@ -405,55 +218,124 @@
     <t>Einarbeitungsphase</t>
   </si>
   <si>
+    <t>Anforderungsanalyse</t>
+  </si>
+  <si>
     <t>Implementierungsphase</t>
   </si>
   <si>
+    <t>Projektplan &amp; Rollenverteilung</t>
+  </si>
+  <si>
+    <t>Recherchebericht</t>
+  </si>
+  <si>
+    <t>Entwurf Interface</t>
+  </si>
+  <si>
+    <t>Pflichtenheft</t>
+  </si>
+  <si>
+    <t>Design-Beschreibung des Produkts</t>
+  </si>
+  <si>
+    <t>Risikoanalyse</t>
+  </si>
+  <si>
+    <t>Einsatzumfeld eines MuD</t>
+  </si>
+  <si>
+    <t>Übersicht MuDs</t>
+  </si>
+  <si>
+    <t>Darstellung der IT-Spezifika fremder MuDs</t>
+  </si>
+  <si>
+    <t>Entwurf Datenhaltung</t>
+  </si>
+  <si>
+    <t>Glossar</t>
+  </si>
+  <si>
+    <t>Testsuiten / ein Testkonzept</t>
+  </si>
+  <si>
     <t>Werkzeug und Git Entscheidung</t>
   </si>
   <si>
-    <t>Projektplan &amp; Rollenverteilung</t>
-  </si>
-  <si>
-    <t>Einsatzumfeld eines MuD</t>
-  </si>
-  <si>
-    <t>Übersicht MuDs</t>
-  </si>
-  <si>
-    <t>Darstellung der IT-Spezifika fremder MuDs</t>
-  </si>
-  <si>
-    <t>Entwurf Interface</t>
-  </si>
-  <si>
-    <t>Entwurf Datenhaltung</t>
-  </si>
-  <si>
-    <t>Anforderungsanalyse</t>
-  </si>
-  <si>
     <t>Lastenheft</t>
   </si>
   <si>
-    <t>Glossar</t>
-  </si>
-  <si>
-    <t>Pflichtenheft</t>
-  </si>
-  <si>
-    <t>Design-Beschreibung des Produkts</t>
-  </si>
-  <si>
-    <t>Testsuiten / ein Testkonzept</t>
-  </si>
-  <si>
     <t>Abgabearchiv</t>
   </si>
   <si>
-    <t>Projektstrukturplan-Artefakt</t>
-  </si>
-  <si>
-    <t>Zusätzliches Artefakt</t>
+    <t>Gruppen Homepage</t>
+  </si>
+  <si>
+    <t>Dokumentations-Richtlinien</t>
+  </si>
+  <si>
+    <t>Designstudie</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mitglied
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Castellar"/>
+      </rPr>
+      <t>Apollon</t>
+    </r>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Rolle</t>
+  </si>
+  <si>
+    <t>Stellvertretend</t>
+  </si>
+  <si>
+    <t>Florian Albert</t>
+  </si>
+  <si>
+    <t>Verantwortlicher für Implementierung</t>
+  </si>
+  <si>
+    <t>Projektleiter</t>
+  </si>
+  <si>
+    <t>Paul-Benedict Burkard</t>
+  </si>
+  <si>
+    <t>Leon Jerke</t>
+  </si>
+  <si>
+    <t>Verantwortlicher für Tests</t>
+  </si>
+  <si>
+    <t>Technischer Assistent / Verantwortlicher für Modellierung</t>
+  </si>
+  <si>
+    <t>Daniel Kröker</t>
+  </si>
+  <si>
+    <t>Qualitätssicherung und Dokumentation</t>
+  </si>
+  <si>
+    <t>Verantwortlicher für Recherche</t>
+  </si>
+  <si>
+    <t>Alfred Rustemi</t>
+  </si>
+  <si>
+    <t>Etienne Zink</t>
   </si>
   <si>
     <r>
@@ -470,6 +352,124 @@
     </r>
   </si>
   <si>
+    <t>Projektstrukturplan-Artefakt</t>
+  </si>
+  <si>
+    <t>Meilensteine</t>
+  </si>
+  <si>
+    <t>Verantwortlich</t>
+  </si>
+  <si>
+    <t>Geschätzter Aufwand</t>
+  </si>
+  <si>
+    <t>Anmerkungen</t>
+  </si>
+  <si>
+    <t>Hochladen?</t>
+  </si>
+  <si>
+    <t>Fertigsgestellt</t>
+  </si>
+  <si>
+    <t>Projektplan</t>
+  </si>
+  <si>
+    <t>Aufsetzen des Projektplans</t>
+  </si>
+  <si>
+    <t>Projektleiter | Paul-Benedict Burkard</t>
+  </si>
+  <si>
+    <t>8h</t>
+  </si>
+  <si>
+    <t>ü</t>
+  </si>
+  <si>
+    <t>Besprechen der Elemente mit dem Team</t>
+  </si>
+  <si>
+    <t>Gesamtes Team</t>
+  </si>
+  <si>
+    <t>Pflegen des Projektplans</t>
+  </si>
+  <si>
+    <t>Kontinuierliche Aufgabe, nicht auf dieses Blatt begrenzt</t>
+  </si>
+  <si>
+    <t>Verantwortlicher für Qualitätssicherung | Daniel Kröker</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>Rollenverteilung</t>
+  </si>
+  <si>
+    <t>30min</t>
+  </si>
+  <si>
+    <t>IDE/UML-Werkzeuge</t>
+  </si>
+  <si>
+    <t>Technischer Assistent | Etienne Zink</t>
+  </si>
+  <si>
+    <t>Mit Betreuer abzusprechen</t>
+  </si>
+  <si>
+    <t>û</t>
+  </si>
+  <si>
+    <t>GIT-Entscheidung</t>
+  </si>
+  <si>
+    <t>Aufsetzen der Homepage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website erstellen: Leon 
+Server hosten: Etienne </t>
+  </si>
+  <si>
+    <t>Tutorial für das Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hochladen aller Artefakte </t>
+  </si>
+  <si>
+    <t>15min</t>
+  </si>
+  <si>
+    <t>Zusätzliches Artefakt</t>
+  </si>
+  <si>
+    <t>SCRUM Dokumentation</t>
+  </si>
+  <si>
+    <t>SCRUM einrichten</t>
+  </si>
+  <si>
+    <t>Verantwortlicher für Implementierung | Florian Albert</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>Gehosted auf GitHub</t>
+  </si>
+  <si>
+    <t>Dokumentation veröffentlichen</t>
+  </si>
+  <si>
+    <t>30h</t>
+  </si>
+  <si>
+    <t>Aufwandsbericht</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Recherchephase
 </t>
@@ -484,72 +484,75 @@
     </r>
   </si>
   <si>
+    <t>Gefordertes Artefakt</t>
+  </si>
+  <si>
+    <t>Verantwortlicher für Recherche | Alfred Rustemi</t>
+  </si>
+  <si>
     <t>Übersicht fremder MuDs</t>
   </si>
   <si>
     <t>Darstellung der IT-Spezifikationen</t>
   </si>
   <si>
-    <t>Verantwortlicher für Recherche | Alfred Rustemi</t>
+    <t>Formulierung des Berichts</t>
   </si>
   <si>
     <t>Entwurf des Interface</t>
   </si>
   <si>
+    <t>Erstellen der Dungeon-Konfiguration</t>
+  </si>
+  <si>
+    <t>20h</t>
+  </si>
+  <si>
+    <t>Verantwortung übernommen von Leon Jerke</t>
+  </si>
+  <si>
+    <t>Erstellen der Spieleansicht</t>
+  </si>
+  <si>
+    <t>Erstellen eines Chatsystems</t>
+  </si>
+  <si>
+    <t>Erstellen einer Login-Systems</t>
+  </si>
+  <si>
+    <t>Erstellen einer Übersichtsseite</t>
+  </si>
+  <si>
     <t>Entwurf der Datenhaltung</t>
   </si>
   <si>
+    <t>10h</t>
+  </si>
+  <si>
+    <t>Entwurf der Spielelogik</t>
+  </si>
+  <si>
     <t>Erste Version des Glossars</t>
   </si>
   <si>
-    <t>Entwurf der Spielelogik</t>
-  </si>
-  <si>
-    <t>10h</t>
-  </si>
-  <si>
-    <t>Designstudie</t>
-  </si>
-  <si>
-    <t>Dokumentations-Richtlinien</t>
-  </si>
-  <si>
     <t>Dokumentationskonzept</t>
   </si>
   <si>
     <t>Verantwortlicher für Qualtitätsmanagement | Daniel Kröker</t>
   </si>
   <si>
-    <t>Erstellen der Dungeon-Konfiguration</t>
-  </si>
-  <si>
-    <t>Erstellen der Spieleansicht</t>
-  </si>
-  <si>
-    <t>Erstellen eines Chatsystems</t>
-  </si>
-  <si>
-    <t>Erstellen einer Übersichtsseite</t>
-  </si>
-  <si>
-    <t>Erstellen einer Login-Systems</t>
-  </si>
-  <si>
-    <t>Verantwortung übernommen von Leon Jerke</t>
-  </si>
-  <si>
     <t>Verantwortlicher für Modellierung | Etienne Zink</t>
   </si>
   <si>
-    <t>20h</t>
-  </si>
-  <si>
     <t>4h</t>
   </si>
   <si>
     <t>Übertragen des Lastenhefts</t>
   </si>
   <si>
+    <t>3h</t>
+  </si>
+  <si>
     <t>Zeichnen der UML-Diagramme</t>
   </si>
   <si>
@@ -559,7 +562,55 @@
     <t>Überarbeitung und Erweiterung des Glossars</t>
   </si>
   <si>
-    <t>3h</t>
+    <t>Implementieren der DTOs</t>
+  </si>
+  <si>
+    <t>15h</t>
+  </si>
+  <si>
+    <t>Erster Schritt</t>
+  </si>
+  <si>
+    <t>Implemetieren des Frontends</t>
+  </si>
+  <si>
+    <t>Implementieren der Razor Components</t>
+  </si>
+  <si>
+    <t>50h</t>
+  </si>
+  <si>
+    <t>Top-Down Implementierung</t>
+  </si>
+  <si>
+    <t>Implementieren der Services</t>
+  </si>
+  <si>
+    <t>Implementieren der SignalR-Schnittstellen</t>
+  </si>
+  <si>
+    <t>5h</t>
+  </si>
+  <si>
+    <t>Implementieren des Backends</t>
+  </si>
+  <si>
+    <t>Implementieren der Modell-Klassen und Datenanbindung</t>
+  </si>
+  <si>
+    <t>70h</t>
+  </si>
+  <si>
+    <t>Bottom-up Implementierung</t>
+  </si>
+  <si>
+    <t>Implementieren der REST-Schnittstellen</t>
+  </si>
+  <si>
+    <t>Implementieren der Service-Klassen</t>
+  </si>
+  <si>
+    <t>60h</t>
   </si>
   <si>
     <t>Testkonzept</t>
@@ -571,64 +622,13 @@
     <t>Design Beschreibung</t>
   </si>
   <si>
-    <t>5h</t>
-  </si>
-  <si>
     <t>35h</t>
   </si>
   <si>
-    <t>Implementieren des Backends</t>
-  </si>
-  <si>
-    <t>Implementieren der DTOs</t>
-  </si>
-  <si>
-    <t>Implemetieren des Frontends</t>
-  </si>
-  <si>
-    <t>Implementieren der Razor Components</t>
-  </si>
-  <si>
-    <t>Implementieren der Services</t>
-  </si>
-  <si>
-    <t>Implementieren der Service-Klassen</t>
-  </si>
-  <si>
-    <t>Implementieren der Modell-Klassen und Datenanbindung</t>
-  </si>
-  <si>
-    <t>Implementieren der REST-Schnittstellen</t>
-  </si>
-  <si>
-    <t>Implementieren der SignalR-Schnittstellen</t>
-  </si>
-  <si>
-    <t>15h</t>
-  </si>
-  <si>
-    <t>50h</t>
-  </si>
-  <si>
-    <t>Erster Schritt</t>
-  </si>
-  <si>
-    <t>70h</t>
-  </si>
-  <si>
-    <t>Top-Down Implementierung</t>
-  </si>
-  <si>
-    <t>Bottom-up Implementierung</t>
-  </si>
-  <si>
-    <t>60h</t>
+    <t>Wöchentlich Updaten</t>
   </si>
   <si>
     <t>Wöchentlich</t>
-  </si>
-  <si>
-    <t>Wöchentlich Updaten</t>
   </si>
 </sst>
 </file>
@@ -2359,7 +2359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="252">
+  <cellXfs count="236">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2577,9 +2577,6 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2709,27 +2706,6 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2880,76 +2856,52 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="111" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="114" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="116" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="111" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="114" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="116" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4937,456 +4889,456 @@
   <sheetData>
     <row r="1" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
-      <c r="B1" s="119"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
       <c r="N1" s="21"/>
       <c r="O1" s="22"/>
     </row>
     <row r="2" spans="1:15" ht="38.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="112"/>
+      <c r="A2" s="111"/>
       <c r="B2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="122"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="101"/>
-      <c r="M2" s="101"/>
-      <c r="N2" s="102"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="101"/>
       <c r="O2" s="28"/>
     </row>
     <row r="3" spans="1:15" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
-      <c r="B3" s="207" t="s">
+      <c r="B3" s="191" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="208"/>
-      <c r="D3" s="209"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="N3" s="102"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="193"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="101"/>
       <c r="O3" s="28"/>
     </row>
     <row r="4" spans="1:15" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="112"/>
-      <c r="B4" s="210" t="s">
+      <c r="A4" s="111"/>
+      <c r="B4" s="194" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="211"/>
-      <c r="D4" s="212"/>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="103"/>
-      <c r="H4" s="103"/>
-      <c r="I4" s="103"/>
-      <c r="J4" s="103"/>
-      <c r="K4" s="103"/>
-      <c r="L4" s="103"/>
-      <c r="M4" s="103"/>
-      <c r="N4" s="103"/>
+      <c r="C4" s="195"/>
+      <c r="D4" s="196"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="102"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="102"/>
+      <c r="N4" s="102"/>
       <c r="O4" s="35"/>
     </row>
     <row r="5" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="112"/>
-      <c r="B5" s="213"/>
-      <c r="C5" s="214"/>
-      <c r="D5" s="215"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="103"/>
-      <c r="J5" s="103"/>
-      <c r="K5" s="103"/>
-      <c r="L5" s="103"/>
-      <c r="M5" s="103"/>
-      <c r="N5" s="103"/>
+      <c r="A5" s="111"/>
+      <c r="B5" s="197"/>
+      <c r="C5" s="198"/>
+      <c r="D5" s="199"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="102"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="102"/>
+      <c r="K5" s="102"/>
+      <c r="L5" s="102"/>
+      <c r="M5" s="102"/>
+      <c r="N5" s="102"/>
       <c r="O5" s="35"/>
     </row>
     <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="112"/>
-      <c r="B6" s="213"/>
-      <c r="C6" s="214"/>
-      <c r="D6" s="215"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="103"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="103"/>
-      <c r="L6" s="103"/>
-      <c r="M6" s="103"/>
-      <c r="N6" s="103"/>
+      <c r="A6" s="111"/>
+      <c r="B6" s="197"/>
+      <c r="C6" s="198"/>
+      <c r="D6" s="199"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="102"/>
+      <c r="H6" s="102"/>
+      <c r="I6" s="102"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="102"/>
+      <c r="M6" s="102"/>
+      <c r="N6" s="102"/>
       <c r="O6" s="35"/>
     </row>
     <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="112"/>
-      <c r="B7" s="213"/>
-      <c r="C7" s="214"/>
-      <c r="D7" s="215"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="103"/>
-      <c r="G7" s="103"/>
-      <c r="H7" s="103"/>
-      <c r="I7" s="103"/>
-      <c r="J7" s="103"/>
-      <c r="K7" s="103"/>
-      <c r="L7" s="103"/>
-      <c r="M7" s="103"/>
-      <c r="N7" s="103"/>
+      <c r="A7" s="111"/>
+      <c r="B7" s="197"/>
+      <c r="C7" s="198"/>
+      <c r="D7" s="199"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="102"/>
+      <c r="I7" s="102"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="102"/>
+      <c r="L7" s="102"/>
+      <c r="M7" s="102"/>
+      <c r="N7" s="102"/>
       <c r="O7" s="35"/>
     </row>
     <row r="8" spans="1:15" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="112"/>
-      <c r="B8" s="213"/>
-      <c r="C8" s="214"/>
-      <c r="D8" s="215"/>
-      <c r="E8" s="103"/>
-      <c r="F8" s="103"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="103"/>
-      <c r="J8" s="103"/>
-      <c r="K8" s="103"/>
-      <c r="L8" s="103"/>
-      <c r="M8" s="103"/>
-      <c r="N8" s="103"/>
+      <c r="A8" s="111"/>
+      <c r="B8" s="197"/>
+      <c r="C8" s="198"/>
+      <c r="D8" s="199"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="102"/>
+      <c r="L8" s="102"/>
+      <c r="M8" s="102"/>
+      <c r="N8" s="102"/>
       <c r="O8" s="35"/>
     </row>
     <row r="9" spans="1:15" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="112"/>
-      <c r="B9" s="216"/>
-      <c r="C9" s="217"/>
-      <c r="D9" s="218"/>
-      <c r="E9" s="103"/>
-      <c r="F9" s="103"/>
-      <c r="G9" s="103"/>
-      <c r="H9" s="103"/>
-      <c r="I9" s="103"/>
-      <c r="J9" s="103"/>
-      <c r="K9" s="103"/>
-      <c r="L9" s="103"/>
-      <c r="M9" s="103"/>
-      <c r="N9" s="103"/>
+      <c r="A9" s="111"/>
+      <c r="B9" s="200"/>
+      <c r="C9" s="201"/>
+      <c r="D9" s="202"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="102"/>
+      <c r="I9" s="102"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="102"/>
+      <c r="L9" s="102"/>
+      <c r="M9" s="102"/>
+      <c r="N9" s="102"/>
       <c r="O9" s="28"/>
     </row>
     <row r="10" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="112"/>
-      <c r="B10" s="116"/>
-      <c r="C10" s="103"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="103"/>
-      <c r="F10" s="103"/>
-      <c r="G10" s="103"/>
-      <c r="H10" s="103"/>
-      <c r="I10" s="103"/>
-      <c r="J10" s="103"/>
-      <c r="K10" s="103"/>
-      <c r="L10" s="103"/>
-      <c r="M10" s="103"/>
-      <c r="N10" s="103"/>
+      <c r="A10" s="111"/>
+      <c r="B10" s="115"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="102"/>
+      <c r="I10" s="102"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="102"/>
+      <c r="M10" s="102"/>
+      <c r="N10" s="102"/>
       <c r="O10" s="35"/>
     </row>
     <row r="11" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="112"/>
-      <c r="B11" s="116"/>
-      <c r="C11" s="103"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="103"/>
-      <c r="G11" s="103"/>
-      <c r="H11" s="103"/>
-      <c r="I11" s="103"/>
-      <c r="J11" s="103"/>
-      <c r="K11" s="103"/>
-      <c r="L11" s="103"/>
-      <c r="M11" s="103"/>
-      <c r="N11" s="103"/>
+      <c r="A11" s="111"/>
+      <c r="B11" s="115"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="102"/>
+      <c r="M11" s="102"/>
+      <c r="N11" s="102"/>
       <c r="O11" s="35"/>
     </row>
     <row r="12" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="112"/>
-      <c r="B12" s="116"/>
-      <c r="C12" s="103"/>
-      <c r="D12" s="103"/>
-      <c r="E12" s="103"/>
-      <c r="F12" s="103"/>
-      <c r="G12" s="103"/>
-      <c r="H12" s="103"/>
-      <c r="I12" s="103"/>
-      <c r="J12" s="103"/>
-      <c r="K12" s="103"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="103"/>
-      <c r="N12" s="103"/>
+      <c r="A12" s="111"/>
+      <c r="B12" s="115"/>
+      <c r="C12" s="102"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102"/>
+      <c r="G12" s="102"/>
+      <c r="H12" s="102"/>
+      <c r="I12" s="102"/>
+      <c r="J12" s="102"/>
+      <c r="K12" s="102"/>
+      <c r="L12" s="102"/>
+      <c r="M12" s="102"/>
+      <c r="N12" s="102"/>
       <c r="O12" s="35"/>
     </row>
     <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="112"/>
-      <c r="B13" s="117"/>
-      <c r="C13" s="103"/>
-      <c r="D13" s="103"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="106"/>
-      <c r="I13" s="107"/>
-      <c r="J13" s="107"/>
-      <c r="K13" s="107"/>
-      <c r="L13" s="107"/>
-      <c r="M13" s="107"/>
-      <c r="N13" s="103"/>
+      <c r="A13" s="111"/>
+      <c r="B13" s="116"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="104"/>
+      <c r="H13" s="105"/>
+      <c r="I13" s="106"/>
+      <c r="J13" s="106"/>
+      <c r="K13" s="106"/>
+      <c r="L13" s="106"/>
+      <c r="M13" s="106"/>
+      <c r="N13" s="102"/>
       <c r="O13" s="35"/>
     </row>
     <row r="14" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="112"/>
-      <c r="B14" s="117"/>
-      <c r="C14" s="103"/>
-      <c r="D14" s="103"/>
-      <c r="E14" s="103"/>
-      <c r="F14" s="107"/>
-      <c r="G14" s="107"/>
-      <c r="H14" s="105"/>
-      <c r="I14" s="104"/>
-      <c r="J14" s="107"/>
-      <c r="K14" s="106"/>
-      <c r="L14" s="107"/>
-      <c r="M14" s="107"/>
-      <c r="N14" s="103"/>
+      <c r="A14" s="111"/>
+      <c r="B14" s="116"/>
+      <c r="C14" s="102"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="106"/>
+      <c r="G14" s="106"/>
+      <c r="H14" s="104"/>
+      <c r="I14" s="103"/>
+      <c r="J14" s="106"/>
+      <c r="K14" s="105"/>
+      <c r="L14" s="106"/>
+      <c r="M14" s="106"/>
+      <c r="N14" s="102"/>
       <c r="O14" s="35"/>
     </row>
     <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="112"/>
-      <c r="B15" s="117"/>
-      <c r="C15" s="103"/>
-      <c r="D15" s="103"/>
-      <c r="E15" s="103"/>
-      <c r="F15" s="107"/>
-      <c r="G15" s="107"/>
-      <c r="H15" s="107"/>
-      <c r="I15" s="107"/>
-      <c r="J15" s="105"/>
-      <c r="K15" s="104"/>
-      <c r="L15" s="107"/>
-      <c r="M15" s="107"/>
-      <c r="N15" s="103"/>
+      <c r="A15" s="111"/>
+      <c r="B15" s="116"/>
+      <c r="C15" s="102"/>
+      <c r="D15" s="102"/>
+      <c r="E15" s="102"/>
+      <c r="F15" s="106"/>
+      <c r="G15" s="106"/>
+      <c r="H15" s="106"/>
+      <c r="I15" s="106"/>
+      <c r="J15" s="104"/>
+      <c r="K15" s="103"/>
+      <c r="L15" s="106"/>
+      <c r="M15" s="106"/>
+      <c r="N15" s="102"/>
       <c r="O15" s="35"/>
     </row>
     <row r="16" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="112"/>
-      <c r="B16" s="117"/>
-      <c r="C16" s="103"/>
-      <c r="D16" s="103"/>
-      <c r="E16" s="103"/>
-      <c r="F16" s="107"/>
-      <c r="G16" s="107"/>
-      <c r="H16" s="107"/>
-      <c r="I16" s="107"/>
-      <c r="J16" s="107"/>
-      <c r="K16" s="107"/>
-      <c r="L16" s="107"/>
-      <c r="M16" s="104"/>
-      <c r="N16" s="103"/>
+      <c r="A16" s="111"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="106"/>
+      <c r="G16" s="106"/>
+      <c r="H16" s="106"/>
+      <c r="I16" s="106"/>
+      <c r="J16" s="106"/>
+      <c r="K16" s="106"/>
+      <c r="L16" s="106"/>
+      <c r="M16" s="103"/>
+      <c r="N16" s="102"/>
       <c r="O16" s="35"/>
     </row>
     <row r="17" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="112"/>
-      <c r="B17" s="118"/>
-      <c r="C17" s="108"/>
-      <c r="D17" s="108"/>
-      <c r="E17" s="108"/>
-      <c r="F17" s="108"/>
-      <c r="G17" s="108"/>
-      <c r="H17" s="108"/>
-      <c r="I17" s="108"/>
-      <c r="J17" s="108"/>
-      <c r="K17" s="108"/>
-      <c r="L17" s="108"/>
-      <c r="M17" s="108"/>
-      <c r="N17" s="109"/>
+      <c r="A17" s="111"/>
+      <c r="B17" s="117"/>
+      <c r="C17" s="107"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="107"/>
+      <c r="H17" s="107"/>
+      <c r="I17" s="107"/>
+      <c r="J17" s="107"/>
+      <c r="K17" s="107"/>
+      <c r="L17" s="107"/>
+      <c r="M17" s="107"/>
+      <c r="N17" s="108"/>
       <c r="O17" s="35"/>
     </row>
     <row r="18" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="112"/>
-      <c r="B18" s="117"/>
-      <c r="C18" s="103"/>
-      <c r="D18" s="103"/>
-      <c r="E18" s="103"/>
-      <c r="F18" s="103"/>
-      <c r="G18" s="103"/>
-      <c r="H18" s="103"/>
-      <c r="I18" s="103"/>
-      <c r="J18" s="103"/>
-      <c r="K18" s="103"/>
-      <c r="L18" s="103"/>
-      <c r="M18" s="103"/>
-      <c r="N18" s="103"/>
+      <c r="A18" s="111"/>
+      <c r="B18" s="116"/>
+      <c r="C18" s="102"/>
+      <c r="D18" s="102"/>
+      <c r="E18" s="102"/>
+      <c r="F18" s="102"/>
+      <c r="G18" s="102"/>
+      <c r="H18" s="102"/>
+      <c r="I18" s="102"/>
+      <c r="J18" s="102"/>
+      <c r="K18" s="102"/>
+      <c r="L18" s="102"/>
+      <c r="M18" s="102"/>
+      <c r="N18" s="102"/>
       <c r="O18" s="35"/>
     </row>
     <row r="19" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="112"/>
-      <c r="B19" s="117"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="106"/>
-      <c r="E19" s="107"/>
-      <c r="F19" s="107"/>
-      <c r="G19" s="107"/>
-      <c r="H19" s="107"/>
-      <c r="I19" s="103"/>
-      <c r="J19" s="103"/>
-      <c r="K19" s="103"/>
-      <c r="L19" s="103"/>
-      <c r="M19" s="103"/>
-      <c r="N19" s="103"/>
+      <c r="A19" s="111"/>
+      <c r="B19" s="116"/>
+      <c r="C19" s="109"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="106"/>
+      <c r="F19" s="106"/>
+      <c r="G19" s="106"/>
+      <c r="H19" s="106"/>
+      <c r="I19" s="102"/>
+      <c r="J19" s="102"/>
+      <c r="K19" s="102"/>
+      <c r="L19" s="102"/>
+      <c r="M19" s="102"/>
+      <c r="N19" s="102"/>
       <c r="O19" s="35"/>
     </row>
     <row r="20" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="112"/>
-      <c r="B20" s="117"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="111"/>
-      <c r="E20" s="106"/>
-      <c r="F20" s="107"/>
-      <c r="G20" s="107"/>
-      <c r="H20" s="107"/>
-      <c r="I20" s="103"/>
-      <c r="J20" s="103"/>
-      <c r="K20" s="103"/>
-      <c r="L20" s="103"/>
-      <c r="M20" s="103"/>
-      <c r="N20" s="103"/>
+      <c r="A20" s="111"/>
+      <c r="B20" s="116"/>
+      <c r="C20" s="102"/>
+      <c r="D20" s="110"/>
+      <c r="E20" s="105"/>
+      <c r="F20" s="106"/>
+      <c r="G20" s="106"/>
+      <c r="H20" s="106"/>
+      <c r="I20" s="102"/>
+      <c r="J20" s="102"/>
+      <c r="K20" s="102"/>
+      <c r="L20" s="102"/>
+      <c r="M20" s="102"/>
+      <c r="N20" s="102"/>
       <c r="O20" s="35"/>
     </row>
     <row r="21" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="112"/>
-      <c r="B21" s="117"/>
-      <c r="C21" s="103"/>
-      <c r="D21" s="106"/>
-      <c r="E21" s="111"/>
-      <c r="F21" s="106"/>
-      <c r="G21" s="106"/>
-      <c r="H21" s="107"/>
-      <c r="I21" s="103"/>
-      <c r="J21" s="103"/>
-      <c r="K21" s="103"/>
-      <c r="L21" s="103"/>
-      <c r="M21" s="103"/>
-      <c r="N21" s="103"/>
+      <c r="A21" s="111"/>
+      <c r="B21" s="116"/>
+      <c r="C21" s="102"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="110"/>
+      <c r="F21" s="105"/>
+      <c r="G21" s="105"/>
+      <c r="H21" s="106"/>
+      <c r="I21" s="102"/>
+      <c r="J21" s="102"/>
+      <c r="K21" s="102"/>
+      <c r="L21" s="102"/>
+      <c r="M21" s="102"/>
+      <c r="N21" s="102"/>
       <c r="O21" s="35"/>
     </row>
     <row r="22" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="112"/>
-      <c r="B22" s="117"/>
-      <c r="C22" s="103"/>
-      <c r="D22" s="107"/>
-      <c r="E22" s="106"/>
-      <c r="F22" s="111"/>
-      <c r="G22" s="106"/>
-      <c r="H22" s="107"/>
-      <c r="I22" s="103"/>
-      <c r="J22" s="103"/>
-      <c r="K22" s="103"/>
-      <c r="L22" s="103"/>
-      <c r="M22" s="103"/>
-      <c r="N22" s="103"/>
+      <c r="A22" s="111"/>
+      <c r="B22" s="116"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="106"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="110"/>
+      <c r="G22" s="105"/>
+      <c r="H22" s="106"/>
+      <c r="I22" s="102"/>
+      <c r="J22" s="102"/>
+      <c r="K22" s="102"/>
+      <c r="L22" s="102"/>
+      <c r="M22" s="102"/>
+      <c r="N22" s="102"/>
       <c r="O22" s="35"/>
     </row>
     <row r="23" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="112"/>
-      <c r="B23" s="117"/>
-      <c r="C23" s="103"/>
-      <c r="D23" s="107"/>
-      <c r="E23" s="107"/>
-      <c r="F23" s="107"/>
-      <c r="G23" s="106"/>
-      <c r="H23" s="111"/>
-      <c r="I23" s="103"/>
-      <c r="J23" s="103"/>
-      <c r="K23" s="103"/>
-      <c r="L23" s="103"/>
-      <c r="M23" s="103"/>
-      <c r="N23" s="103"/>
+      <c r="A23" s="111"/>
+      <c r="B23" s="116"/>
+      <c r="C23" s="102"/>
+      <c r="D23" s="106"/>
+      <c r="E23" s="106"/>
+      <c r="F23" s="106"/>
+      <c r="G23" s="105"/>
+      <c r="H23" s="110"/>
+      <c r="I23" s="102"/>
+      <c r="J23" s="102"/>
+      <c r="K23" s="102"/>
+      <c r="L23" s="102"/>
+      <c r="M23" s="102"/>
+      <c r="N23" s="102"/>
       <c r="O23" s="35"/>
     </row>
     <row r="24" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="112"/>
-      <c r="B24" s="117"/>
-      <c r="C24" s="103"/>
-      <c r="D24" s="103"/>
-      <c r="E24" s="103"/>
-      <c r="F24" s="103"/>
-      <c r="G24" s="103"/>
-      <c r="H24" s="103"/>
-      <c r="I24" s="103"/>
-      <c r="J24" s="103"/>
-      <c r="K24" s="103"/>
-      <c r="L24" s="103"/>
-      <c r="M24" s="103"/>
-      <c r="N24" s="103"/>
+      <c r="A24" s="111"/>
+      <c r="B24" s="116"/>
+      <c r="C24" s="102"/>
+      <c r="D24" s="102"/>
+      <c r="E24" s="102"/>
+      <c r="F24" s="102"/>
+      <c r="G24" s="102"/>
+      <c r="H24" s="102"/>
+      <c r="I24" s="102"/>
+      <c r="J24" s="102"/>
+      <c r="K24" s="102"/>
+      <c r="L24" s="102"/>
+      <c r="M24" s="102"/>
+      <c r="N24" s="102"/>
       <c r="O24" s="35"/>
     </row>
     <row r="25" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="112"/>
-      <c r="B25" s="117"/>
-      <c r="C25" s="103"/>
-      <c r="D25" s="103"/>
-      <c r="E25" s="103"/>
-      <c r="F25" s="103"/>
-      <c r="G25" s="103"/>
-      <c r="H25" s="103"/>
-      <c r="I25" s="103"/>
-      <c r="J25" s="103"/>
-      <c r="K25" s="103"/>
-      <c r="L25" s="103"/>
-      <c r="M25" s="103"/>
-      <c r="N25" s="103"/>
+      <c r="A25" s="111"/>
+      <c r="B25" s="116"/>
+      <c r="C25" s="102"/>
+      <c r="D25" s="102"/>
+      <c r="E25" s="102"/>
+      <c r="F25" s="102"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="102"/>
+      <c r="I25" s="102"/>
+      <c r="J25" s="102"/>
+      <c r="K25" s="102"/>
+      <c r="L25" s="102"/>
+      <c r="M25" s="102"/>
+      <c r="N25" s="102"/>
       <c r="O25" s="35"/>
     </row>
     <row r="26" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="112"/>
-      <c r="B26" s="117"/>
-      <c r="C26" s="103"/>
-      <c r="D26" s="103"/>
-      <c r="E26" s="103"/>
-      <c r="F26" s="103"/>
-      <c r="G26" s="103"/>
-      <c r="H26" s="103"/>
-      <c r="I26" s="103"/>
-      <c r="J26" s="103"/>
-      <c r="K26" s="103"/>
-      <c r="L26" s="103"/>
-      <c r="M26" s="103"/>
-      <c r="N26" s="110"/>
+      <c r="A26" s="111"/>
+      <c r="B26" s="116"/>
+      <c r="C26" s="102"/>
+      <c r="D26" s="102"/>
+      <c r="E26" s="102"/>
+      <c r="F26" s="102"/>
+      <c r="G26" s="102"/>
+      <c r="H26" s="102"/>
+      <c r="I26" s="102"/>
+      <c r="J26" s="102"/>
+      <c r="K26" s="102"/>
+      <c r="L26" s="102"/>
+      <c r="M26" s="102"/>
+      <c r="N26" s="109"/>
       <c r="O26" s="22"/>
     </row>
     <row r="27" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="113"/>
-      <c r="B27" s="103"/>
-      <c r="C27" s="115"/>
+      <c r="A27" s="112"/>
+      <c r="B27" s="102"/>
+      <c r="C27" s="114"/>
       <c r="D27" s="47"/>
       <c r="E27" s="47"/>
       <c r="F27" s="47"/>
@@ -5400,8 +5352,8 @@
       <c r="N27" s="47"/>
     </row>
     <row r="28" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="114"/>
-      <c r="B28" s="103"/>
+      <c r="A28" s="113"/>
+      <c r="B28" s="102"/>
       <c r="C28" s="22"/>
     </row>
     <row r="29" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -5424,7 +5376,7 @@
   <dimension ref="A1:AB41"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5520,7 +5472,7 @@
     </row>
     <row r="3" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29"/>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="97" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="30"/>
@@ -5539,10 +5491,10 @@
     </row>
     <row r="4" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24"/>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="99"/>
+      <c r="C4" s="98"/>
       <c r="D4" s="4"/>
       <c r="E4" s="33"/>
       <c r="F4" s="33"/>
@@ -5558,7 +5510,7 @@
     </row>
     <row r="5" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24"/>
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="96" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="36"/>
@@ -5577,7 +5529,7 @@
     </row>
     <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="24"/>
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="96" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="38"/>
@@ -5596,7 +5548,7 @@
     </row>
     <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="24"/>
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="96" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="38"/>
@@ -5615,7 +5567,7 @@
     </row>
     <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="24"/>
-      <c r="B8" s="97" t="s">
+      <c r="B8" s="96" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="38"/>
@@ -5634,7 +5586,7 @@
     </row>
     <row r="9" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="96" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="39"/>
@@ -5653,7 +5605,7 @@
     </row>
     <row r="10" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="24"/>
-      <c r="B10" s="97" t="s">
+      <c r="B10" s="96" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="39"/>
@@ -5672,7 +5624,7 @@
     </row>
     <row r="11" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="24"/>
-      <c r="B11" s="97" t="s">
+      <c r="B11" s="96" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="39"/>
@@ -5798,16 +5750,16 @@
         <v>30</v>
       </c>
       <c r="C17" s="7"/>
-      <c r="D17" s="123"/>
-      <c r="E17" s="123"/>
-      <c r="F17" s="123"/>
-      <c r="G17" s="123"/>
-      <c r="H17" s="123"/>
-      <c r="I17" s="123"/>
-      <c r="J17" s="123"/>
-      <c r="K17" s="123"/>
-      <c r="L17" s="123"/>
-      <c r="M17" s="123"/>
+      <c r="D17" s="184"/>
+      <c r="E17" s="184"/>
+      <c r="F17" s="184"/>
+      <c r="G17" s="184"/>
+      <c r="H17" s="184"/>
+      <c r="I17" s="184"/>
+      <c r="J17" s="184"/>
+      <c r="K17" s="184"/>
+      <c r="L17" s="184"/>
+      <c r="M17" s="184"/>
       <c r="N17" s="14" t="s">
         <v>31</v>
       </c>
@@ -5835,7 +5787,7 @@
     <row r="19" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="24"/>
       <c r="B19" s="9" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="C19" s="12">
         <v>44269</v>
@@ -5856,7 +5808,7 @@
     <row r="20" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="24"/>
       <c r="B20" s="9" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="C20" s="38"/>
       <c r="D20" s="13">
@@ -5877,7 +5829,7 @@
     <row r="21" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="24"/>
       <c r="B21" s="9" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="C21" s="38"/>
       <c r="D21" s="5"/>
@@ -5898,7 +5850,7 @@
     <row r="22" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24"/>
       <c r="B22" s="9" t="s">
-        <v>96</v>
+        <v>36</v>
       </c>
       <c r="C22" s="38"/>
       <c r="D22" s="6"/>
@@ -5919,7 +5871,7 @@
     <row r="23" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="24"/>
       <c r="B23" s="9" t="s">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="C23" s="38"/>
       <c r="D23" s="6"/>
@@ -5940,7 +5892,7 @@
     <row r="24" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24"/>
       <c r="B24" s="9" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="C24" s="38"/>
       <c r="D24" s="33"/>
@@ -5958,7 +5910,7 @@
         <v>44325</v>
       </c>
       <c r="L24" s="13">
-        <v>44363</v>
+        <v>44332</v>
       </c>
       <c r="M24" s="33"/>
       <c r="N24" s="34"/>
@@ -5967,7 +5919,7 @@
     <row r="25" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24"/>
       <c r="B25" s="10" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C25" s="40"/>
       <c r="D25" s="41"/>
@@ -5986,7 +5938,7 @@
     <row r="26" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="24"/>
       <c r="B26" s="11" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C26" s="45"/>
       <c r="D26" s="46"/>
@@ -6083,234 +6035,234 @@
   <sheetData>
     <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F3" s="130"/>
-      <c r="G3" s="130"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
     </row>
     <row r="4" spans="1:13" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="157"/>
-      <c r="E4" s="156"/>
-      <c r="F4" s="219" t="s">
-        <v>99</v>
-      </c>
-      <c r="G4" s="220"/>
-      <c r="H4" s="178"/>
-      <c r="I4" s="157"/>
-      <c r="J4" s="157"/>
+      <c r="D4" s="149"/>
+      <c r="E4" s="148"/>
+      <c r="F4" s="203" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="204"/>
+      <c r="H4" s="170"/>
+      <c r="I4" s="149"/>
+      <c r="J4" s="149"/>
     </row>
     <row r="5" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="159"/>
-      <c r="C5" s="179"/>
-      <c r="D5" s="158"/>
-      <c r="E5" s="132"/>
-      <c r="F5" s="132"/>
-      <c r="G5" s="132"/>
-      <c r="H5" s="132"/>
-      <c r="I5" s="132"/>
-      <c r="J5" s="177"/>
-      <c r="K5" s="176"/>
-      <c r="L5" s="157"/>
+      <c r="B5" s="151"/>
+      <c r="C5" s="171"/>
+      <c r="D5" s="150"/>
+      <c r="E5" s="124"/>
+      <c r="F5" s="124"/>
+      <c r="G5" s="124"/>
+      <c r="H5" s="124"/>
+      <c r="I5" s="124"/>
+      <c r="J5" s="169"/>
+      <c r="K5" s="168"/>
+      <c r="L5" s="149"/>
     </row>
     <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="114"/>
-      <c r="B6" s="160"/>
-      <c r="C6" s="131"/>
-      <c r="D6" s="131"/>
-      <c r="E6" s="131"/>
-      <c r="F6" s="131"/>
-      <c r="G6" s="131"/>
-      <c r="H6" s="131"/>
-      <c r="I6" s="131"/>
-      <c r="J6" s="148"/>
-      <c r="K6" s="131"/>
-      <c r="L6" s="175"/>
+      <c r="A6" s="113"/>
+      <c r="B6" s="152"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="123"/>
+      <c r="I6" s="123"/>
+      <c r="J6" s="140"/>
+      <c r="K6" s="123"/>
+      <c r="L6" s="167"/>
       <c r="M6" s="22"/>
     </row>
     <row r="7" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="114"/>
-      <c r="B7" s="161" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="146"/>
-      <c r="D7" s="221" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" s="222"/>
-      <c r="F7" s="223"/>
-      <c r="G7" s="146"/>
-      <c r="H7" s="145" t="s">
-        <v>102</v>
-      </c>
-      <c r="I7" s="147"/>
-      <c r="J7" s="145" t="s">
-        <v>111</v>
-      </c>
-      <c r="K7" s="146"/>
-      <c r="L7" s="170" t="s">
-        <v>103</v>
+      <c r="A7" s="113"/>
+      <c r="B7" s="153" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="138"/>
+      <c r="D7" s="205" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="206"/>
+      <c r="F7" s="207"/>
+      <c r="G7" s="138"/>
+      <c r="H7" s="137" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="139"/>
+      <c r="J7" s="137" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="138"/>
+      <c r="L7" s="162" t="s">
+        <v>46</v>
       </c>
       <c r="M7" s="22"/>
     </row>
     <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="114"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="135"/>
-      <c r="E8" s="135"/>
-      <c r="F8" s="135"/>
-      <c r="G8" s="134"/>
-      <c r="H8" s="134"/>
-      <c r="I8" s="134"/>
-      <c r="J8" s="134"/>
-      <c r="L8" s="166"/>
+      <c r="A8" s="113"/>
+      <c r="B8" s="154"/>
+      <c r="C8" s="125"/>
+      <c r="D8" s="127"/>
+      <c r="E8" s="127"/>
+      <c r="F8" s="127"/>
+      <c r="G8" s="126"/>
+      <c r="H8" s="126"/>
+      <c r="I8" s="126"/>
+      <c r="J8" s="126"/>
+      <c r="L8" s="158"/>
       <c r="M8" s="22"/>
     </row>
     <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="114"/>
-      <c r="B9" s="163"/>
-      <c r="C9" s="137"/>
-      <c r="D9" s="142"/>
-      <c r="E9" s="142"/>
-      <c r="F9" s="142"/>
-      <c r="G9" s="136"/>
-      <c r="H9" s="135"/>
-      <c r="I9" s="134"/>
-      <c r="J9" s="135"/>
-      <c r="L9" s="171"/>
+      <c r="A9" s="113"/>
+      <c r="B9" s="155"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="134"/>
+      <c r="E9" s="134"/>
+      <c r="F9" s="134"/>
+      <c r="G9" s="128"/>
+      <c r="H9" s="127"/>
+      <c r="I9" s="126"/>
+      <c r="J9" s="127"/>
+      <c r="L9" s="163"/>
       <c r="M9" s="22"/>
     </row>
     <row r="10" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="166"/>
-      <c r="B10" s="164" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="139"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="144" t="s">
-        <v>90</v>
-      </c>
-      <c r="F10" s="143"/>
-      <c r="G10" s="139"/>
-      <c r="H10" s="138" t="s">
-        <v>109</v>
-      </c>
-      <c r="I10" s="139"/>
-      <c r="J10" s="138" t="s">
-        <v>114</v>
-      </c>
-      <c r="K10" s="141"/>
-      <c r="L10" s="172" t="s">
-        <v>115</v>
+      <c r="A10" s="158"/>
+      <c r="B10" s="156" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="131"/>
+      <c r="D10" s="113"/>
+      <c r="E10" s="136" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="135"/>
+      <c r="G10" s="131"/>
+      <c r="H10" s="130" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="131"/>
+      <c r="J10" s="130" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="133"/>
+      <c r="L10" s="164" t="s">
+        <v>51</v>
       </c>
       <c r="M10" s="22"/>
     </row>
     <row r="11" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="166"/>
-      <c r="B11" s="165"/>
-      <c r="C11" s="134"/>
-      <c r="D11" s="140"/>
-      <c r="E11" s="140"/>
-      <c r="F11" s="140"/>
-      <c r="G11" s="134"/>
-      <c r="H11" s="140"/>
-      <c r="I11" s="134"/>
-      <c r="J11" s="133"/>
-      <c r="L11" s="173"/>
+      <c r="A11" s="158"/>
+      <c r="B11" s="157"/>
+      <c r="C11" s="126"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="132"/>
+      <c r="F11" s="132"/>
+      <c r="G11" s="126"/>
+      <c r="H11" s="132"/>
+      <c r="I11" s="126"/>
+      <c r="J11" s="125"/>
+      <c r="L11" s="165"/>
       <c r="M11" s="22"/>
     </row>
     <row r="12" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="166"/>
-      <c r="B12" s="164" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="137"/>
-      <c r="D12" s="138" t="s">
-        <v>106</v>
-      </c>
-      <c r="E12" s="138" t="s">
-        <v>107</v>
-      </c>
-      <c r="F12" s="138" t="s">
-        <v>108</v>
-      </c>
-      <c r="G12" s="139"/>
-      <c r="H12" s="138" t="s">
-        <v>110</v>
-      </c>
-      <c r="I12" s="136"/>
-      <c r="J12" s="138" t="s">
-        <v>113</v>
-      </c>
-      <c r="K12" s="114"/>
-      <c r="L12" s="172" t="s">
-        <v>116</v>
+      <c r="A12" s="158"/>
+      <c r="B12" s="156" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="129"/>
+      <c r="D12" s="130" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="130" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="130" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="131"/>
+      <c r="H12" s="130" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="128"/>
+      <c r="J12" s="130" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" s="113"/>
+      <c r="L12" s="164" t="s">
+        <v>58</v>
       </c>
       <c r="M12" s="22"/>
     </row>
     <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="166"/>
-      <c r="B13" s="136"/>
-      <c r="C13" s="134"/>
-      <c r="D13" s="133"/>
-      <c r="E13" s="133"/>
-      <c r="F13" s="133"/>
-      <c r="G13" s="134"/>
-      <c r="H13" s="140"/>
-      <c r="I13" s="134"/>
-      <c r="J13" s="134"/>
-      <c r="L13" s="173"/>
+      <c r="A13" s="158"/>
+      <c r="B13" s="128"/>
+      <c r="C13" s="126"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="125"/>
+      <c r="F13" s="125"/>
+      <c r="G13" s="126"/>
+      <c r="H13" s="132"/>
+      <c r="I13" s="126"/>
+      <c r="J13" s="126"/>
+      <c r="L13" s="165"/>
       <c r="M13" s="22"/>
     </row>
     <row r="14" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="166"/>
-      <c r="B14" s="164" t="s">
-        <v>104</v>
-      </c>
-      <c r="C14" s="134"/>
-      <c r="D14" s="134"/>
-      <c r="E14" s="134"/>
-      <c r="F14" s="134"/>
-      <c r="G14" s="137"/>
-      <c r="H14" s="138" t="s">
-        <v>112</v>
-      </c>
-      <c r="I14" s="136"/>
-      <c r="J14" s="134"/>
-      <c r="K14" s="114"/>
-      <c r="L14" s="172" t="s">
-        <v>117</v>
+      <c r="A14" s="158"/>
+      <c r="B14" s="156" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="126"/>
+      <c r="D14" s="126"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="126"/>
+      <c r="G14" s="129"/>
+      <c r="H14" s="130" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="128"/>
+      <c r="J14" s="126"/>
+      <c r="K14" s="113"/>
+      <c r="L14" s="164" t="s">
+        <v>61</v>
       </c>
       <c r="M14" s="22"/>
     </row>
     <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="166"/>
-      <c r="B15" s="136"/>
-      <c r="C15" s="134"/>
-      <c r="D15" s="134"/>
-      <c r="E15" s="134"/>
-      <c r="F15" s="134"/>
-      <c r="G15" s="134"/>
-      <c r="H15" s="140"/>
-      <c r="I15" s="134"/>
-      <c r="J15" s="134"/>
-      <c r="L15" s="174"/>
+      <c r="A15" s="158"/>
+      <c r="B15" s="128"/>
+      <c r="C15" s="126"/>
+      <c r="D15" s="126"/>
+      <c r="E15" s="126"/>
+      <c r="F15" s="126"/>
+      <c r="G15" s="126"/>
+      <c r="H15" s="132"/>
+      <c r="I15" s="126"/>
+      <c r="J15" s="126"/>
+      <c r="L15" s="166"/>
       <c r="M15" s="22"/>
     </row>
     <row r="16" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="166"/>
-      <c r="B16" s="192" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="114"/>
-      <c r="H16" s="194" t="s">
-        <v>131</v>
-      </c>
-      <c r="L16" s="171"/>
+      <c r="A16" s="158"/>
+      <c r="B16" s="177" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="113"/>
+      <c r="H16" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="L16" s="163"/>
       <c r="M16" s="22"/>
     </row>
     <row r="17" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="187"/>
-      <c r="B17" s="188"/>
-      <c r="C17" s="189"/>
+      <c r="A17" s="172"/>
+      <c r="B17" s="173"/>
+      <c r="C17" s="174"/>
       <c r="D17" s="47"/>
       <c r="E17" s="47"/>
       <c r="F17" s="47"/>
@@ -6319,45 +6271,45 @@
       <c r="I17" s="47"/>
       <c r="J17" s="47"/>
       <c r="K17" s="47"/>
-      <c r="L17" s="171"/>
+      <c r="L17" s="163"/>
     </row>
     <row r="18" spans="1:22" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="187"/>
-      <c r="B18" s="190"/>
-      <c r="C18" s="191"/>
-      <c r="D18" s="167"/>
-      <c r="E18" s="167"/>
-      <c r="F18" s="167"/>
-      <c r="G18" s="168"/>
-      <c r="H18" s="193" t="s">
-        <v>130</v>
-      </c>
-      <c r="I18" s="169"/>
-      <c r="J18" s="167"/>
-      <c r="K18" s="157"/>
-      <c r="L18" s="156"/>
+      <c r="A18" s="172"/>
+      <c r="B18" s="175"/>
+      <c r="C18" s="176"/>
+      <c r="D18" s="159"/>
+      <c r="E18" s="159"/>
+      <c r="F18" s="159"/>
+      <c r="G18" s="160"/>
+      <c r="H18" s="178" t="s">
+        <v>64</v>
+      </c>
+      <c r="I18" s="161"/>
+      <c r="J18" s="159"/>
+      <c r="K18" s="149"/>
+      <c r="L18" s="148"/>
     </row>
     <row r="20" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="130"/>
+      <c r="C20" s="122"/>
     </row>
     <row r="21" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="47"/>
     </row>
     <row r="30" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U30" s="130"/>
-      <c r="V30" s="130"/>
+      <c r="U30" s="122"/>
+      <c r="V30" s="122"/>
     </row>
     <row r="31" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="15:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P33" s="114"/>
+      <c r="P33" s="113"/>
       <c r="AB33" s="22"/>
     </row>
     <row r="34" spans="15:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O34" s="48"/>
-      <c r="P34" s="114"/>
+      <c r="P34" s="113"/>
     </row>
     <row r="37" spans="15:28" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P37" s="114"/>
+      <c r="P37" s="113"/>
       <c r="AB37" s="22"/>
     </row>
     <row r="39" spans="15:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6367,15 +6319,15 @@
       <c r="AB41" s="22"/>
     </row>
     <row r="44" spans="15:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Q44" s="134"/>
-      <c r="R44" s="134"/>
-      <c r="S44" s="134"/>
-      <c r="T44" s="134"/>
-      <c r="U44" s="134"/>
-      <c r="V44" s="134"/>
-      <c r="W44" s="133"/>
-      <c r="X44" s="134"/>
-      <c r="Y44" s="134"/>
+      <c r="Q44" s="126"/>
+      <c r="R44" s="126"/>
+      <c r="S44" s="126"/>
+      <c r="T44" s="126"/>
+      <c r="U44" s="126"/>
+      <c r="V44" s="126"/>
+      <c r="W44" s="125"/>
+      <c r="X44" s="126"/>
+      <c r="Y44" s="126"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6412,7 +6364,7 @@
     <row r="2" spans="1:27" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="49"/>
       <c r="B2" s="60" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="C2" s="61"/>
       <c r="D2" s="62"/>
@@ -6443,13 +6395,13 @@
     <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="49"/>
       <c r="B3" s="65" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="C3" s="63" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="D3" s="64" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="E3" s="50"/>
       <c r="F3" s="17"/>
@@ -6477,14 +6429,14 @@
     </row>
     <row r="4" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="49"/>
-      <c r="B4" s="90" t="s">
-        <v>39</v>
+      <c r="B4" s="89" t="s">
+        <v>69</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D4" s="55" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="E4" s="50"/>
       <c r="F4" s="17"/>
@@ -6512,14 +6464,14 @@
     </row>
     <row r="5" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="49"/>
-      <c r="B5" s="90" t="s">
-        <v>42</v>
+      <c r="B5" s="89" t="s">
+        <v>72</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="D5" s="55" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E5" s="50"/>
       <c r="F5" s="17"/>
@@ -6547,14 +6499,14 @@
     </row>
     <row r="6" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="49"/>
-      <c r="B6" s="90" t="s">
-        <v>43</v>
+      <c r="B6" s="89" t="s">
+        <v>73</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="D6" s="56" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="E6" s="50"/>
       <c r="F6" s="17"/>
@@ -6582,14 +6534,14 @@
     </row>
     <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="49"/>
-      <c r="B7" s="90" t="s">
-        <v>46</v>
+      <c r="B7" s="89" t="s">
+        <v>76</v>
       </c>
       <c r="C7" s="57" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="D7" s="56" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="E7" s="50"/>
       <c r="F7" s="17"/>
@@ -6617,14 +6569,14 @@
     </row>
     <row r="8" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="49"/>
-      <c r="B8" s="90" t="s">
-        <v>49</v>
+      <c r="B8" s="89" t="s">
+        <v>79</v>
       </c>
       <c r="C8" s="57" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="D8" s="56" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="E8" s="50"/>
       <c r="F8" s="17"/>
@@ -6652,14 +6604,14 @@
     </row>
     <row r="9" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="49"/>
-      <c r="B9" s="91" t="s">
-        <v>50</v>
+      <c r="B9" s="90" t="s">
+        <v>80</v>
       </c>
       <c r="C9" s="58" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="E9" s="50"/>
       <c r="F9" s="17"/>
@@ -8276,322 +8228,322 @@
     <row r="2" spans="1:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="71"/>
       <c r="B2" s="75" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="84"/>
+        <v>81</v>
+      </c>
+      <c r="C2" s="80"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="83"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="71"/>
-      <c r="B3" s="80" t="s">
-        <v>118</v>
+      <c r="B3" s="79" t="s">
+        <v>82</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="D3" s="76" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="E3" s="76" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="F3" s="76" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="G3" s="76" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="H3" s="78" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71"/>
-      <c r="B4" s="228" t="s">
-        <v>58</v>
+      <c r="B4" s="212" t="s">
+        <v>89</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="123" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="231" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" s="123"/>
-      <c r="G4" s="232" t="s">
-        <v>62</v>
-      </c>
-      <c r="H4" s="233" t="s">
-        <v>62</v>
+        <v>90</v>
+      </c>
+      <c r="D4" s="184" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="215" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="184"/>
+      <c r="G4" s="216" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="217" t="s">
+        <v>93</v>
       </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
-      <c r="B5" s="229"/>
+      <c r="B5" s="213"/>
       <c r="C5" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="123" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="231"/>
-      <c r="F5" s="123"/>
-      <c r="G5" s="232"/>
-      <c r="H5" s="233"/>
+        <v>94</v>
+      </c>
+      <c r="D5" s="184" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="215"/>
+      <c r="F5" s="184"/>
+      <c r="G5" s="216"/>
+      <c r="H5" s="217"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="71"/>
-      <c r="B6" s="230"/>
+      <c r="B6" s="214"/>
       <c r="C6" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="123" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="231"/>
-      <c r="F6" s="123" t="s">
-        <v>66</v>
-      </c>
-      <c r="G6" s="232"/>
-      <c r="H6" s="233"/>
+        <v>96</v>
+      </c>
+      <c r="D6" s="184" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="215"/>
+      <c r="F6" s="184" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="216"/>
+      <c r="H6" s="217"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="71"/>
-      <c r="B7" s="126" t="s">
-        <v>67</v>
+      <c r="B7" s="190" t="s">
+        <v>52</v>
       </c>
       <c r="C7" s="7"/>
-      <c r="D7" s="123" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="123" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="123"/>
-      <c r="G7" s="124" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" s="129" t="s">
-        <v>62</v>
+      <c r="D7" s="184" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="184" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" s="184"/>
+      <c r="G7" s="185" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" s="186" t="s">
+        <v>93</v>
       </c>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="71"/>
-      <c r="B8" s="126" t="s">
-        <v>70</v>
+      <c r="B8" s="190" t="s">
+        <v>100</v>
       </c>
       <c r="C8" s="7"/>
-      <c r="D8" s="123" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="123" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" s="123"/>
-      <c r="G8" s="124" t="s">
-        <v>62</v>
-      </c>
-      <c r="H8" s="125" t="s">
-        <v>62</v>
+      <c r="D8" s="184" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="184" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="184"/>
+      <c r="G8" s="185" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" s="186" t="s">
+        <v>93</v>
       </c>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="71"/>
-      <c r="B9" s="79" t="s">
-        <v>72</v>
+      <c r="B9" s="187" t="s">
+        <v>102</v>
       </c>
       <c r="C9" s="7"/>
-      <c r="D9" s="123" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="123" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="123" t="s">
-        <v>74</v>
-      </c>
-      <c r="G9" s="124" t="s">
-        <v>75</v>
-      </c>
-      <c r="H9" s="129" t="s">
-        <v>62</v>
+      <c r="D9" s="184" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="184" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="184" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="185" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" s="186" t="s">
+        <v>93</v>
       </c>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="71"/>
-      <c r="B10" s="126" t="s">
-        <v>76</v>
+      <c r="B10" s="190" t="s">
+        <v>106</v>
       </c>
       <c r="C10" s="7"/>
-      <c r="D10" s="123" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="123" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="123" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="124" t="s">
-        <v>75</v>
-      </c>
-      <c r="H10" s="129" t="s">
-        <v>62</v>
+      <c r="D10" s="184" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="184" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="184" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" s="185" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="186" t="s">
+        <v>93</v>
       </c>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="71"/>
-      <c r="B11" s="234" t="s">
-        <v>84</v>
+      <c r="B11" s="218" t="s">
+        <v>62</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="238" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="127" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="127" t="s">
-        <v>86</v>
-      </c>
-      <c r="G11" s="128"/>
-      <c r="H11" s="129" t="s">
-        <v>62</v>
+        <v>107</v>
+      </c>
+      <c r="D11" s="222" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="184" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="184" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" s="185"/>
+      <c r="H11" s="186" t="s">
+        <v>93</v>
       </c>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="71"/>
-      <c r="B12" s="236"/>
+      <c r="B12" s="220"/>
       <c r="C12" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" s="239"/>
-      <c r="E12" s="127" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="127"/>
-      <c r="G12" s="128" t="s">
-        <v>75</v>
-      </c>
-      <c r="H12" s="129" t="s">
-        <v>62</v>
+        <v>109</v>
+      </c>
+      <c r="D12" s="223"/>
+      <c r="E12" s="184" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="184"/>
+      <c r="G12" s="185" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12" s="186" t="s">
+        <v>93</v>
       </c>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="71"/>
-      <c r="B13" s="237"/>
-      <c r="C13" s="127" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="240"/>
-      <c r="E13" s="127" t="s">
-        <v>89</v>
-      </c>
-      <c r="F13" s="127"/>
-      <c r="G13" s="128" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="129" t="s">
-        <v>62</v>
+      <c r="B13" s="221"/>
+      <c r="C13" s="184" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="224"/>
+      <c r="E13" s="184" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" s="184"/>
+      <c r="G13" s="185" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" s="186" t="s">
+        <v>93</v>
       </c>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="71"/>
-      <c r="B14" s="150" t="s">
+      <c r="B14" s="142" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="143" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="141" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="141" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="141" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="225" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="226"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="218" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="184" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="184" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" s="184" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" s="210" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="211"/>
+    </row>
+    <row r="16" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="219"/>
+      <c r="C16" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="184" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="184" t="s">
         <v>119</v>
       </c>
-      <c r="C14" s="151" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="149" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="149" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="149" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="241" t="s">
-        <v>57</v>
-      </c>
-      <c r="H14" s="242"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="234" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="123" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="123" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="123" t="s">
-        <v>81</v>
-      </c>
-      <c r="G15" s="226" t="s">
-        <v>62</v>
-      </c>
-      <c r="H15" s="227"/>
-    </row>
-    <row r="16" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="235"/>
-      <c r="C16" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" s="123" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="123" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" s="123"/>
-      <c r="G16" s="226" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" s="227"/>
+      <c r="F16" s="184"/>
+      <c r="G16" s="210" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="211"/>
     </row>
     <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="153" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="154"/>
-      <c r="D17" s="155" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="155" t="s">
-        <v>71</v>
-      </c>
-      <c r="F17" s="155"/>
-      <c r="G17" s="224" t="s">
-        <v>75</v>
-      </c>
-      <c r="H17" s="225"/>
+      <c r="B17" s="145" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" s="146"/>
+      <c r="D17" s="147" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" s="147" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" s="147"/>
+      <c r="G17" s="208" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" s="209"/>
     </row>
     <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
@@ -8624,7 +8576,7 @@
     </row>
     <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G24" s="69"/>
-      <c r="H24" s="152"/>
+      <c r="H24" s="144"/>
     </row>
     <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G25" s="69"/>
@@ -8720,166 +8672,166 @@
       <c r="B2" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="94"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="93"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="71"/>
-      <c r="B3" s="95" t="s">
-        <v>51</v>
+      <c r="B3" s="94" t="s">
+        <v>122</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="D3" s="76" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="E3" s="76" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="F3" s="76" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="G3" s="76" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="H3" s="78" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="71"/>
-      <c r="B4" s="243" t="s">
-        <v>90</v>
+      <c r="B4" s="227" t="s">
+        <v>48</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="123" t="s">
-        <v>124</v>
-      </c>
-      <c r="E4" s="123"/>
-      <c r="F4" s="123"/>
-      <c r="G4" s="232" t="s">
-        <v>62</v>
-      </c>
-      <c r="H4" s="180" t="s">
-        <v>62</v>
+        <v>53</v>
+      </c>
+      <c r="D4" s="184" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="184"/>
+      <c r="F4" s="184"/>
+      <c r="G4" s="216" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="186" t="s">
+        <v>93</v>
       </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
-      <c r="B5" s="243"/>
+      <c r="B5" s="227"/>
       <c r="C5" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" s="127" t="s">
         <v>124</v>
       </c>
-      <c r="E5" s="123"/>
-      <c r="F5" s="123"/>
-      <c r="G5" s="232"/>
-      <c r="H5" s="180" t="s">
-        <v>62</v>
+      <c r="D5" s="184" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="184"/>
+      <c r="F5" s="184"/>
+      <c r="G5" s="216"/>
+      <c r="H5" s="186" t="s">
+        <v>93</v>
       </c>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="71"/>
-      <c r="B6" s="243"/>
+      <c r="B6" s="227"/>
       <c r="C6" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="184" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="127" t="s">
-        <v>124</v>
-      </c>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="232"/>
-      <c r="H6" s="180" t="s">
-        <v>62</v>
+      <c r="E6" s="184"/>
+      <c r="F6" s="184"/>
+      <c r="G6" s="216"/>
+      <c r="H6" s="186" t="s">
+        <v>93</v>
       </c>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="71"/>
-      <c r="B7" s="243"/>
+      <c r="B7" s="227"/>
       <c r="C7" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="127" t="s">
-        <v>124</v>
-      </c>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123"/>
-      <c r="G7" s="232"/>
-      <c r="H7" s="180" t="s">
-        <v>62</v>
+        <v>126</v>
+      </c>
+      <c r="D7" s="184" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="184"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="216"/>
+      <c r="H7" s="186" t="s">
+        <v>93</v>
       </c>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="71"/>
-      <c r="B8" s="150" t="s">
-        <v>119</v>
-      </c>
-      <c r="C8" s="151" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="149" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="149" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="149" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="241" t="s">
-        <v>57</v>
-      </c>
-      <c r="H8" s="242"/>
+      <c r="B8" s="142" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="143" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="141" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="141" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="141" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="225" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="226"/>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="71"/>
-      <c r="B9" s="153" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9" s="154"/>
-      <c r="D9" s="155" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="155" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="155"/>
-      <c r="G9" s="224" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" s="225"/>
+      <c r="B9" s="145" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="146"/>
+      <c r="D9" s="147" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="147" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="147"/>
+      <c r="G9" s="208" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" s="209"/>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="87"/>
+      <c r="B10" s="86"/>
       <c r="C10" s="72"/>
-      <c r="D10" s="88"/>
+      <c r="D10" s="87"/>
       <c r="E10" s="2"/>
       <c r="F10" s="72"/>
-      <c r="G10" s="89"/>
+      <c r="G10" s="88"/>
       <c r="H10" s="74"/>
     </row>
     <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="86"/>
+      <c r="B11" s="85"/>
       <c r="C11" s="66"/>
-      <c r="D11" s="85"/>
+      <c r="D11" s="84"/>
       <c r="F11" s="66"/>
       <c r="G11" s="67"/>
       <c r="H11" s="68"/>
@@ -9013,282 +8965,282 @@
       <c r="B2" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="94"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="93"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="71"/>
-      <c r="B3" s="95" t="s">
-        <v>51</v>
+      <c r="B3" s="94" t="s">
+        <v>122</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="D3" s="76" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="E3" s="76" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="F3" s="76" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="G3" s="76" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="H3" s="78" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="71"/>
-      <c r="B4" s="234" t="s">
-        <v>125</v>
+      <c r="B4" s="218" t="s">
+        <v>127</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D4" s="238" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="238" t="s">
-        <v>141</v>
-      </c>
-      <c r="F4" s="238" t="s">
-        <v>139</v>
-      </c>
-      <c r="G4" s="246" t="s">
-        <v>62</v>
-      </c>
-      <c r="H4" s="200" t="s">
-        <v>62</v>
+        <v>128</v>
+      </c>
+      <c r="D4" s="222" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="222" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="222" t="s">
+        <v>130</v>
+      </c>
+      <c r="G4" s="230" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="185" t="s">
+        <v>93</v>
       </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
-      <c r="B5" s="236"/>
+      <c r="B5" s="220"/>
       <c r="C5" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" s="239"/>
-      <c r="E5" s="239"/>
-      <c r="F5" s="239"/>
-      <c r="G5" s="247"/>
-      <c r="H5" s="200" t="s">
-        <v>62</v>
+        <v>131</v>
+      </c>
+      <c r="D5" s="223"/>
+      <c r="E5" s="223"/>
+      <c r="F5" s="223"/>
+      <c r="G5" s="231"/>
+      <c r="H5" s="185" t="s">
+        <v>93</v>
       </c>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="71"/>
-      <c r="B6" s="236"/>
+      <c r="B6" s="220"/>
       <c r="C6" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D6" s="239"/>
-      <c r="E6" s="239"/>
-      <c r="F6" s="239"/>
-      <c r="G6" s="247"/>
-      <c r="H6" s="200" t="s">
-        <v>62</v>
+        <v>132</v>
+      </c>
+      <c r="D6" s="223"/>
+      <c r="E6" s="223"/>
+      <c r="F6" s="223"/>
+      <c r="G6" s="231"/>
+      <c r="H6" s="185" t="s">
+        <v>93</v>
       </c>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="71"/>
-      <c r="B7" s="236"/>
+      <c r="B7" s="220"/>
       <c r="C7" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D7" s="239"/>
-      <c r="E7" s="239"/>
-      <c r="F7" s="239"/>
-      <c r="G7" s="247"/>
-      <c r="H7" s="200" t="s">
-        <v>62</v>
+        <v>133</v>
+      </c>
+      <c r="D7" s="223"/>
+      <c r="E7" s="223"/>
+      <c r="F7" s="223"/>
+      <c r="G7" s="231"/>
+      <c r="H7" s="185" t="s">
+        <v>93</v>
       </c>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="71"/>
-      <c r="B8" s="235"/>
+      <c r="B8" s="219"/>
       <c r="C8" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D8" s="245"/>
-      <c r="E8" s="245"/>
-      <c r="F8" s="245"/>
-      <c r="G8" s="248"/>
-      <c r="H8" s="200" t="s">
-        <v>62</v>
+        <v>134</v>
+      </c>
+      <c r="D8" s="229"/>
+      <c r="E8" s="229"/>
+      <c r="F8" s="229"/>
+      <c r="G8" s="232"/>
+      <c r="H8" s="185" t="s">
+        <v>93</v>
       </c>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="71"/>
-      <c r="B9" s="181" t="s">
-        <v>126</v>
+      <c r="B9" s="190" t="s">
+        <v>135</v>
       </c>
       <c r="C9" s="7"/>
-      <c r="D9" s="127" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="127" t="s">
-        <v>129</v>
-      </c>
-      <c r="F9" s="127"/>
-      <c r="G9" s="183" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" s="200" t="s">
-        <v>62</v>
+      <c r="D9" s="184" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="184" t="s">
+        <v>136</v>
+      </c>
+      <c r="F9" s="184"/>
+      <c r="G9" s="185" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" s="185" t="s">
+        <v>93</v>
       </c>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="71"/>
-      <c r="B10" s="185" t="s">
-        <v>128</v>
+      <c r="B10" s="190" t="s">
+        <v>137</v>
       </c>
       <c r="C10" s="7"/>
-      <c r="D10" s="182" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" s="182" t="s">
-        <v>83</v>
-      </c>
-      <c r="F10" s="182"/>
-      <c r="G10" s="183"/>
-      <c r="H10" s="200" t="s">
-        <v>62</v>
+      <c r="D10" s="184" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="184" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" s="184"/>
+      <c r="G10" s="185"/>
+      <c r="H10" s="185" t="s">
+        <v>93</v>
       </c>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="71"/>
-      <c r="B11" s="181" t="s">
-        <v>127</v>
+      <c r="B11" s="190" t="s">
+        <v>138</v>
       </c>
       <c r="C11" s="7"/>
-      <c r="D11" s="127" t="s">
-        <v>124</v>
-      </c>
-      <c r="E11" s="127" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="127"/>
-      <c r="G11" s="128" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" s="200" t="s">
-        <v>62</v>
+      <c r="D11" s="184" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" s="184" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="184"/>
+      <c r="G11" s="185" t="s">
+        <v>93</v>
+      </c>
+      <c r="H11" s="185" t="s">
+        <v>93</v>
       </c>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="71"/>
-      <c r="B12" s="185" t="s">
-        <v>132</v>
+      <c r="B12" s="190" t="s">
+        <v>139</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="182" t="s">
-        <v>133</v>
-      </c>
-      <c r="E12" s="182" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="182"/>
-      <c r="G12" s="183" t="s">
-        <v>62</v>
-      </c>
-      <c r="H12" s="200" t="s">
-        <v>62</v>
+      <c r="D12" s="184" t="s">
+        <v>140</v>
+      </c>
+      <c r="E12" s="184" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="184"/>
+      <c r="G12" s="185" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="185" t="s">
+        <v>93</v>
       </c>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="71"/>
-      <c r="B13" s="185" t="s">
-        <v>130</v>
+      <c r="B13" s="190" t="s">
+        <v>64</v>
       </c>
       <c r="C13" s="7"/>
-      <c r="D13" s="184" t="s">
-        <v>140</v>
-      </c>
-      <c r="E13" s="184" t="s">
+      <c r="D13" s="188" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="188" t="s">
         <v>142</v>
       </c>
-      <c r="F13" s="184"/>
-      <c r="G13" s="183" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="200" t="s">
-        <v>62</v>
+      <c r="F13" s="188"/>
+      <c r="G13" s="185" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" s="185" t="s">
+        <v>93</v>
       </c>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="71"/>
-      <c r="B14" s="150" t="s">
-        <v>119</v>
-      </c>
-      <c r="C14" s="195" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="197" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="197" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="197" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="244" t="s">
-        <v>57</v>
-      </c>
-      <c r="H14" s="242"/>
+      <c r="B14" s="142" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="180" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="182" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="182" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="182" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="228" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="226"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="71"/>
-      <c r="B15" s="153" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" s="154"/>
-      <c r="D15" s="196" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="196" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="196"/>
-      <c r="G15" s="224" t="s">
-        <v>62</v>
-      </c>
-      <c r="H15" s="225"/>
+      <c r="B15" s="145" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" s="146"/>
+      <c r="D15" s="181" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="181" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="181"/>
+      <c r="G15" s="208" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="209"/>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="87"/>
+      <c r="B16" s="86"/>
       <c r="C16" s="72"/>
-      <c r="D16" s="88"/>
+      <c r="D16" s="87"/>
       <c r="E16" s="2"/>
       <c r="F16" s="72"/>
-      <c r="G16" s="89"/>
+      <c r="G16" s="88"/>
       <c r="H16" s="74"/>
     </row>
     <row r="17" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="86"/>
+      <c r="B17" s="85"/>
       <c r="C17" s="66"/>
-      <c r="D17" s="85"/>
+      <c r="D17" s="84"/>
       <c r="F17" s="66"/>
       <c r="G17" s="67"/>
       <c r="H17" s="68"/>
@@ -9452,174 +9404,174 @@
       <c r="B2" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="94"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="93"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="71"/>
-      <c r="B3" s="95" t="s">
-        <v>51</v>
+      <c r="B3" s="94" t="s">
+        <v>122</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="D3" s="76" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="E3" s="76" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="F3" s="76" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="G3" s="76" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="H3" s="78" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71"/>
-      <c r="B4" s="234" t="s">
-        <v>114</v>
+      <c r="B4" s="218" t="s">
+        <v>50</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>143</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F4" s="7"/>
-      <c r="G4" s="246" t="s">
-        <v>62</v>
-      </c>
-      <c r="H4" s="249" t="s">
-        <v>62</v>
+      <c r="G4" s="230" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="233" t="s">
+        <v>93</v>
       </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
-      <c r="B5" s="236"/>
+      <c r="B5" s="220"/>
       <c r="C5" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="F5" s="7"/>
-      <c r="G5" s="247"/>
-      <c r="H5" s="250"/>
+      <c r="G5" s="231"/>
+      <c r="H5" s="234"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="71"/>
-      <c r="B6" s="236"/>
+      <c r="B6" s="220"/>
       <c r="C6" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="F6" s="7"/>
-      <c r="G6" s="248"/>
-      <c r="H6" s="251"/>
+      <c r="G6" s="232"/>
+      <c r="H6" s="235"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="71"/>
-      <c r="B7" s="186" t="s">
-        <v>113</v>
+      <c r="B7" s="190" t="s">
+        <v>57</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7" s="198" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" s="198" t="s">
-        <v>62</v>
+      <c r="G7" s="183" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" s="183" t="s">
+        <v>93</v>
       </c>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="71"/>
-      <c r="B8" s="150" t="s">
-        <v>119</v>
-      </c>
-      <c r="C8" s="195" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="197" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="197" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="197" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="244" t="s">
-        <v>57</v>
-      </c>
-      <c r="H8" s="242"/>
+      <c r="B8" s="142" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="180" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="182" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="182" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="182" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="228" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="226"/>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="71"/>
-      <c r="B9" s="153" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9" s="154"/>
-      <c r="D9" s="196" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="196" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="196"/>
-      <c r="G9" s="224" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" s="225"/>
+      <c r="B9" s="145" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="146"/>
+      <c r="D9" s="181" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="181" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="181"/>
+      <c r="G9" s="208" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" s="209"/>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="87"/>
+      <c r="B10" s="86"/>
       <c r="C10" s="72"/>
-      <c r="D10" s="88"/>
+      <c r="D10" s="87"/>
       <c r="E10" s="2"/>
       <c r="F10" s="72"/>
-      <c r="G10" s="89"/>
+      <c r="G10" s="88"/>
       <c r="H10" s="74"/>
     </row>
     <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="86"/>
+      <c r="B11" s="85"/>
       <c r="C11" s="66"/>
-      <c r="D11" s="85"/>
+      <c r="D11" s="84"/>
       <c r="F11" s="66"/>
       <c r="G11" s="67"/>
       <c r="H11" s="68"/>
@@ -9751,7 +9703,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9781,290 +9733,290 @@
       <c r="B2" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="94"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="93"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="71"/>
-      <c r="B3" s="95" t="s">
-        <v>51</v>
+      <c r="B3" s="94" t="s">
+        <v>122</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="D3" s="76" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="E3" s="76" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="F3" s="76" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="G3" s="76" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="H3" s="78" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="71"/>
-      <c r="B4" s="206" t="s">
-        <v>154</v>
+      <c r="B4" s="190" t="s">
+        <v>148</v>
       </c>
       <c r="C4" s="7"/>
-      <c r="D4" s="238" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="204" t="s">
-        <v>162</v>
-      </c>
-      <c r="F4" s="204" t="s">
-        <v>164</v>
-      </c>
-      <c r="G4" s="246" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" s="201" t="s">
-        <v>75</v>
+      <c r="D4" s="222" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="188" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" s="188" t="s">
+        <v>150</v>
+      </c>
+      <c r="G4" s="230" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" s="186" t="s">
+        <v>105</v>
       </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
-      <c r="B5" s="234" t="s">
-        <v>155</v>
+      <c r="B5" s="218" t="s">
+        <v>151</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="D5" s="239"/>
-      <c r="E5" s="205" t="s">
-        <v>163</v>
-      </c>
-      <c r="F5" s="239" t="s">
-        <v>166</v>
-      </c>
-      <c r="G5" s="247"/>
-      <c r="H5" s="203" t="s">
-        <v>75</v>
+        <v>152</v>
+      </c>
+      <c r="D5" s="223"/>
+      <c r="E5" s="189" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" s="223" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" s="231"/>
+      <c r="H5" s="186" t="s">
+        <v>105</v>
       </c>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="71"/>
-      <c r="B6" s="236"/>
+      <c r="B6" s="220"/>
       <c r="C6" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="D6" s="239"/>
-      <c r="E6" s="205" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="239"/>
-      <c r="G6" s="247"/>
-      <c r="H6" s="201" t="s">
-        <v>75</v>
+        <v>155</v>
+      </c>
+      <c r="D6" s="223"/>
+      <c r="E6" s="189" t="s">
+        <v>119</v>
+      </c>
+      <c r="F6" s="223"/>
+      <c r="G6" s="231"/>
+      <c r="H6" s="186" t="s">
+        <v>105</v>
       </c>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="71"/>
-      <c r="B7" s="235"/>
+      <c r="B7" s="219"/>
       <c r="C7" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="D7" s="239"/>
-      <c r="E7" s="205" t="s">
-        <v>151</v>
-      </c>
-      <c r="F7" s="239"/>
-      <c r="G7" s="247"/>
-      <c r="H7" s="203" t="s">
-        <v>75</v>
+        <v>156</v>
+      </c>
+      <c r="D7" s="223"/>
+      <c r="E7" s="189" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7" s="223"/>
+      <c r="G7" s="231"/>
+      <c r="H7" s="186" t="s">
+        <v>105</v>
       </c>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="71"/>
-      <c r="B8" s="234" t="s">
-        <v>153</v>
+      <c r="B8" s="218" t="s">
+        <v>158</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="D8" s="239"/>
-      <c r="E8" s="205" t="s">
-        <v>165</v>
-      </c>
-      <c r="F8" s="239" t="s">
-        <v>167</v>
-      </c>
-      <c r="G8" s="247"/>
-      <c r="H8" s="203" t="s">
-        <v>75</v>
+      <c r="D8" s="223"/>
+      <c r="E8" s="189" t="s">
+        <v>160</v>
+      </c>
+      <c r="F8" s="223" t="s">
+        <v>161</v>
+      </c>
+      <c r="G8" s="231"/>
+      <c r="H8" s="186" t="s">
+        <v>105</v>
       </c>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="71"/>
-      <c r="B9" s="236"/>
+      <c r="B9" s="220"/>
       <c r="C9" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="D9" s="239"/>
-      <c r="E9" s="205" t="s">
-        <v>129</v>
-      </c>
-      <c r="F9" s="239"/>
-      <c r="G9" s="247"/>
-      <c r="H9" s="203" t="s">
-        <v>75</v>
+        <v>156</v>
+      </c>
+      <c r="D9" s="223"/>
+      <c r="E9" s="189" t="s">
+        <v>136</v>
+      </c>
+      <c r="F9" s="223"/>
+      <c r="G9" s="231"/>
+      <c r="H9" s="186" t="s">
+        <v>105</v>
       </c>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="71"/>
-      <c r="B10" s="236"/>
+      <c r="B10" s="220"/>
       <c r="C10" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="D10" s="239"/>
-      <c r="E10" s="205" t="s">
-        <v>83</v>
-      </c>
-      <c r="F10" s="239"/>
-      <c r="G10" s="247"/>
-      <c r="H10" s="203" t="s">
-        <v>75</v>
+        <v>162</v>
+      </c>
+      <c r="D10" s="223"/>
+      <c r="E10" s="189" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" s="223"/>
+      <c r="G10" s="231"/>
+      <c r="H10" s="186" t="s">
+        <v>105</v>
       </c>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="71"/>
-      <c r="B11" s="235"/>
+      <c r="B11" s="219"/>
       <c r="C11" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="D11" s="239"/>
-      <c r="E11" s="205" t="s">
-        <v>168</v>
-      </c>
-      <c r="F11" s="245"/>
-      <c r="G11" s="247"/>
-      <c r="H11" s="201" t="s">
-        <v>75</v>
+        <v>163</v>
+      </c>
+      <c r="D11" s="223"/>
+      <c r="E11" s="189" t="s">
+        <v>164</v>
+      </c>
+      <c r="F11" s="229"/>
+      <c r="G11" s="231"/>
+      <c r="H11" s="186" t="s">
+        <v>105</v>
       </c>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="71"/>
-      <c r="B12" s="202" t="s">
-        <v>148</v>
+      <c r="B12" s="190" t="s">
+        <v>165</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="199" t="s">
-        <v>149</v>
-      </c>
-      <c r="E12" s="199" t="s">
-        <v>129</v>
-      </c>
-      <c r="F12" s="199"/>
-      <c r="G12" s="200" t="s">
-        <v>62</v>
-      </c>
-      <c r="H12" s="201" t="s">
-        <v>75</v>
+      <c r="D12" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="E12" s="184" t="s">
+        <v>136</v>
+      </c>
+      <c r="F12" s="184"/>
+      <c r="G12" s="185" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="186" t="s">
+        <v>105</v>
       </c>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="71"/>
-      <c r="B13" s="202" t="s">
-        <v>150</v>
+      <c r="B13" s="190" t="s">
+        <v>167</v>
       </c>
       <c r="C13" s="7"/>
-      <c r="D13" s="199" t="s">
-        <v>140</v>
-      </c>
-      <c r="E13" s="199" t="s">
-        <v>152</v>
-      </c>
-      <c r="F13" s="199" t="s">
-        <v>170</v>
-      </c>
-      <c r="G13" s="200" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="201" t="s">
-        <v>75</v>
+      <c r="D13" s="184" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="184" t="s">
+        <v>168</v>
+      </c>
+      <c r="F13" s="184" t="s">
+        <v>169</v>
+      </c>
+      <c r="G13" s="185" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" s="186" t="s">
+        <v>105</v>
       </c>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="71"/>
-      <c r="B14" s="150" t="s">
-        <v>119</v>
-      </c>
-      <c r="C14" s="195" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="197" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="197" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="197" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="244" t="s">
-        <v>57</v>
-      </c>
-      <c r="H14" s="242"/>
+      <c r="B14" s="142" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="180" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="182" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="182" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="182" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="228" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="226"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="71"/>
-      <c r="B15" s="153" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" s="154"/>
-      <c r="D15" s="196" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="196" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="196" t="s">
-        <v>169</v>
-      </c>
-      <c r="G15" s="224" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" s="225"/>
+      <c r="B15" s="145" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" s="146"/>
+      <c r="D15" s="181" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="181" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="181" t="s">
+        <v>170</v>
+      </c>
+      <c r="G15" s="208" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" s="209"/>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="87"/>
+      <c r="B16" s="86"/>
       <c r="C16" s="72"/>
-      <c r="D16" s="88"/>
+      <c r="D16" s="87"/>
       <c r="E16" s="2"/>
       <c r="F16" s="72"/>
-      <c r="G16" s="89"/>
+      <c r="G16" s="88"/>
       <c r="H16" s="74"/>
     </row>
     <row r="17" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="86"/>
+      <c r="B17" s="85"/>
       <c r="C17" s="66"/>
-      <c r="D17" s="85"/>
+      <c r="D17" s="84"/>
       <c r="F17" s="66"/>
       <c r="G17" s="67"/>
       <c r="H17" s="68"/>
@@ -10402,15 +10354,8 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50F9D30A-50A2-408B-B3F0-EDB4CF8C0B75}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9261f3b7-eb37-44bc-ab49-41e0f5c5a530"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>